<commit_message>
Update result values in report metrics
</commit_message>
<xml_diff>
--- a/download/Metrics report.xlsx
+++ b/download/Metrics report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="17">
   <si>
     <t xml:space="preserve">CostQoS – No Adaption</t>
   </si>
@@ -61,28 +61,32 @@
     <t xml:space="preserve">Performance Influence Adapt</t>
   </si>
   <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">Average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="0.00%"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="&quot;BOOL&quot;e&quot;AN&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="0.00%"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -185,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +242,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,15 +262,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,15 +282,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,11 +298,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,11 +329,11 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="R35 E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB4" activeCellId="0" sqref="AB4:AB33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18"/>
@@ -507,34 +515,38 @@
         <f aca="false">(L4/D4)*100</f>
         <v>100</v>
       </c>
-      <c r="R4" s="9"/>
+      <c r="R4" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="13" t="n">
+      <c r="T4" s="14" t="n">
         <v>86</v>
       </c>
-      <c r="U4" s="13" t="n">
+      <c r="U4" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="V4" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W4" s="15" t="n">
+      <c r="V4" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W4" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X4" s="16" t="n">
+      <c r="X4" s="17" t="n">
         <v>39.5348</v>
       </c>
-      <c r="Y4" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z4" s="13" t="n">
+      <c r="Y4" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z4" s="14" t="n">
         <v>0.2093</v>
       </c>
       <c r="AA4" s="9" t="n">
         <f aca="false">(V4/D4)*100</f>
         <v>100</v>
       </c>
-      <c r="AB4" s="13"/>
+      <c r="AB4" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
@@ -587,34 +599,38 @@
         <f aca="false">(L5/D5)*100</f>
         <v>100</v>
       </c>
-      <c r="R5" s="9"/>
+      <c r="R5" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="13" t="n">
+      <c r="T5" s="14" t="n">
         <v>87</v>
       </c>
-      <c r="U5" s="13" t="n">
+      <c r="U5" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="V5" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W5" s="15" t="n">
+      <c r="V5" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W5" s="16" t="n">
         <v>14</v>
       </c>
-      <c r="X5" s="16" t="n">
+      <c r="X5" s="17" t="n">
         <v>41.954</v>
       </c>
-      <c r="Y5" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z5" s="13" t="n">
+      <c r="Y5" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z5" s="14" t="n">
         <v>0.1609</v>
       </c>
       <c r="AA5" s="9" t="n">
         <f aca="false">(V5/D5)*100</f>
         <v>100</v>
       </c>
-      <c r="AB5" s="13"/>
+      <c r="AB5" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
@@ -667,34 +683,38 @@
         <f aca="false">(L6/D6)*100</f>
         <v>100</v>
       </c>
-      <c r="R6" s="9"/>
+      <c r="R6" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="13" t="n">
+      <c r="T6" s="14" t="n">
         <v>89</v>
       </c>
-      <c r="U6" s="13" t="n">
+      <c r="U6" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="V6" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W6" s="15" t="n">
+      <c r="V6" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W6" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X6" s="16" t="n">
+      <c r="X6" s="17" t="n">
         <v>41.0112</v>
       </c>
-      <c r="Y6" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z6" s="13" t="n">
+      <c r="Y6" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="14" t="n">
         <v>0.1797</v>
       </c>
       <c r="AA6" s="9" t="n">
         <f aca="false">(V6/D6)*100</f>
         <v>100</v>
       </c>
-      <c r="AB6" s="13"/>
+      <c r="AB6" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="n">
@@ -747,34 +767,38 @@
         <f aca="false">(L7/D7)*100</f>
         <v>100</v>
       </c>
-      <c r="R7" s="9"/>
+      <c r="R7" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S7" s="1"/>
-      <c r="T7" s="13" t="n">
+      <c r="T7" s="14" t="n">
         <v>88</v>
       </c>
-      <c r="U7" s="13" t="n">
+      <c r="U7" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="V7" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W7" s="15" t="n">
+      <c r="V7" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W7" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X7" s="16" t="n">
+      <c r="X7" s="17" t="n">
         <v>40.3409</v>
       </c>
-      <c r="Y7" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z7" s="13" t="n">
+      <c r="Y7" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z7" s="14" t="n">
         <v>0.1931</v>
       </c>
       <c r="AA7" s="9" t="n">
         <f aca="false">(V7/D7)*100</f>
         <v>100</v>
       </c>
-      <c r="AB7" s="13"/>
+      <c r="AB7" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="n">
@@ -827,34 +851,38 @@
         <f aca="false">(L8/D8)*100</f>
         <v>100</v>
       </c>
-      <c r="R8" s="9"/>
+      <c r="R8" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S8" s="1"/>
-      <c r="T8" s="13" t="n">
+      <c r="T8" s="14" t="n">
         <v>98</v>
       </c>
-      <c r="U8" s="13" t="n">
+      <c r="U8" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="V8" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W8" s="15" t="n">
+      <c r="V8" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W8" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X8" s="16" t="n">
+      <c r="X8" s="17" t="n">
         <v>39.2857</v>
       </c>
-      <c r="Y8" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z8" s="13" t="n">
+      <c r="Y8" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z8" s="14" t="n">
         <v>0.2142</v>
       </c>
       <c r="AA8" s="9" t="n">
         <f aca="false">(V8/D8)*100</f>
         <v>100</v>
       </c>
-      <c r="AB8" s="13"/>
+      <c r="AB8" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
@@ -907,34 +935,38 @@
         <f aca="false">(L9/D9)*100</f>
         <v>100</v>
       </c>
-      <c r="R9" s="9"/>
+      <c r="R9" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S9" s="1"/>
-      <c r="T9" s="13" t="n">
+      <c r="T9" s="14" t="n">
         <v>91</v>
       </c>
-      <c r="U9" s="13" t="n">
+      <c r="U9" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="V9" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W9" s="15" t="n">
+      <c r="V9" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W9" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X9" s="16" t="n">
+      <c r="X9" s="17" t="n">
         <v>39.5604</v>
       </c>
-      <c r="Y9" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z9" s="13" t="n">
+      <c r="Y9" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="14" t="n">
         <v>0.2087</v>
       </c>
       <c r="AA9" s="9" t="n">
         <f aca="false">(V9/D9)*100</f>
         <v>100</v>
       </c>
-      <c r="AB9" s="13"/>
+      <c r="AB9" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="n">
@@ -987,34 +1019,38 @@
         <f aca="false">(L10/D10)*100</f>
         <v>100</v>
       </c>
-      <c r="R10" s="9"/>
+      <c r="R10" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S10" s="1"/>
-      <c r="T10" s="13" t="n">
+      <c r="T10" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U10" s="13" t="n">
+      <c r="U10" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="V10" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W10" s="15" t="n">
+      <c r="V10" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W10" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X10" s="16" t="n">
+      <c r="X10" s="17" t="n">
         <v>41.3043</v>
       </c>
-      <c r="Y10" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z10" s="13" t="n">
+      <c r="Y10" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z10" s="14" t="n">
         <v>0.1739</v>
       </c>
       <c r="AA10" s="9" t="n">
         <f aca="false">(V10/D10)*100</f>
         <v>100</v>
       </c>
-      <c r="AB10" s="13"/>
+      <c r="AB10" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="n">
@@ -1067,34 +1103,38 @@
         <f aca="false">(L11/D11)*100</f>
         <v>100</v>
       </c>
-      <c r="R11" s="9"/>
+      <c r="R11" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S11" s="1"/>
-      <c r="T11" s="13" t="n">
+      <c r="T11" s="14" t="n">
         <v>90</v>
       </c>
-      <c r="U11" s="13" t="n">
+      <c r="U11" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="V11" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W11" s="15" t="n">
+      <c r="V11" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W11" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X11" s="16" t="n">
+      <c r="X11" s="17" t="n">
         <v>44.4444</v>
       </c>
-      <c r="Y11" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z11" s="13" t="n">
+      <c r="Y11" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z11" s="14" t="n">
         <v>0.1111</v>
       </c>
       <c r="AA11" s="9" t="n">
         <f aca="false">(V11/D11)*100</f>
         <v>100</v>
       </c>
-      <c r="AB11" s="13"/>
+      <c r="AB11" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
@@ -1112,7 +1152,7 @@
       <c r="E12" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="F12" s="17" t="n">
+      <c r="F12" s="18" t="n">
         <v>43.75</v>
       </c>
       <c r="G12" s="11" t="n">
@@ -1134,7 +1174,7 @@
       <c r="M12" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="N12" s="17" t="n">
+      <c r="N12" s="18" t="n">
         <v>41.8478</v>
       </c>
       <c r="O12" s="11" t="n">
@@ -1147,34 +1187,38 @@
         <f aca="false">(L12/D12)*100</f>
         <v>100</v>
       </c>
-      <c r="R12" s="9"/>
+      <c r="R12" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S12" s="1"/>
-      <c r="T12" s="13" t="n">
+      <c r="T12" s="14" t="n">
         <v>91</v>
       </c>
-      <c r="U12" s="13" t="n">
+      <c r="U12" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="V12" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W12" s="15" t="n">
+      <c r="V12" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W12" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X12" s="16" t="n">
+      <c r="X12" s="17" t="n">
         <v>44.5054</v>
       </c>
-      <c r="Y12" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z12" s="13" t="n">
+      <c r="Y12" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z12" s="14" t="n">
         <v>0.1098</v>
       </c>
       <c r="AA12" s="9" t="n">
         <f aca="false">(V12/D12)*100</f>
         <v>100</v>
       </c>
-      <c r="AB12" s="13"/>
+      <c r="AB12" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
@@ -1227,34 +1271,38 @@
         <f aca="false">(L13/D13)*100</f>
         <v>100</v>
       </c>
-      <c r="R13" s="9"/>
+      <c r="R13" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S13" s="1"/>
-      <c r="T13" s="13" t="n">
+      <c r="T13" s="14" t="n">
         <v>95</v>
       </c>
-      <c r="U13" s="13" t="n">
+      <c r="U13" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="V13" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W13" s="15" t="n">
+      <c r="V13" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W13" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X13" s="16" t="n">
+      <c r="X13" s="17" t="n">
         <v>42.1875</v>
       </c>
-      <c r="Y13" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z13" s="13" t="n">
+      <c r="Y13" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z13" s="14" t="n">
         <v>0.1562</v>
       </c>
       <c r="AA13" s="9" t="n">
         <f aca="false">(V13/D13)*100</f>
         <v>100</v>
       </c>
-      <c r="AB13" s="13"/>
+      <c r="AB13" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="n">
@@ -1307,34 +1355,38 @@
         <f aca="false">(L14/D14)*100</f>
         <v>100</v>
       </c>
-      <c r="R14" s="9"/>
+      <c r="R14" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S14" s="1"/>
-      <c r="T14" s="13" t="n">
+      <c r="T14" s="14" t="n">
         <v>84</v>
       </c>
-      <c r="U14" s="13" t="n">
+      <c r="U14" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="V14" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W14" s="15" t="n">
+      <c r="V14" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W14" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X14" s="16" t="n">
+      <c r="X14" s="17" t="n">
         <v>40.4761</v>
       </c>
-      <c r="Y14" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z14" s="13" t="n">
+      <c r="Y14" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z14" s="14" t="n">
         <v>0.1904</v>
       </c>
       <c r="AA14" s="9" t="n">
         <f aca="false">(V14/D14)*100</f>
         <v>100</v>
       </c>
-      <c r="AB14" s="13"/>
+      <c r="AB14" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="n">
@@ -1387,34 +1439,38 @@
         <f aca="false">(L15/D15)*100</f>
         <v>100</v>
       </c>
-      <c r="R15" s="9"/>
+      <c r="R15" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S15" s="1"/>
-      <c r="T15" s="13" t="n">
+      <c r="T15" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U15" s="13" t="n">
+      <c r="U15" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="V15" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W15" s="15" t="n">
+      <c r="V15" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W15" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X15" s="16" t="n">
+      <c r="X15" s="17" t="n">
         <v>40.7608</v>
       </c>
-      <c r="Y15" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z15" s="13" t="n">
+      <c r="Y15" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z15" s="14" t="n">
         <v>0.1847</v>
       </c>
       <c r="AA15" s="9" t="n">
         <f aca="false">(V15/D15)*100</f>
         <v>100</v>
       </c>
-      <c r="AB15" s="13"/>
+      <c r="AB15" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="n">
@@ -1442,59 +1498,63 @@
         <v>0.2266</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="13" t="n">
+      <c r="J16" s="14" t="n">
         <v>82</v>
       </c>
-      <c r="K16" s="13" t="n">
+      <c r="K16" s="14" t="n">
         <v>13</v>
       </c>
       <c r="L16" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M16" s="15" t="n">
+      <c r="M16" s="16" t="n">
         <v>26.5</v>
       </c>
-      <c r="N16" s="16" t="n">
+      <c r="N16" s="17" t="n">
         <v>42.0731</v>
       </c>
       <c r="O16" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P16" s="13" t="n">
+      <c r="P16" s="14" t="n">
         <v>0.1585</v>
       </c>
       <c r="Q16" s="9" t="n">
         <f aca="false">(L16/D16)*100</f>
         <v>100</v>
       </c>
-      <c r="R16" s="9"/>
+      <c r="R16" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S16" s="1"/>
-      <c r="T16" s="13" t="n">
+      <c r="T16" s="14" t="n">
         <v>90</v>
       </c>
-      <c r="U16" s="13" t="n">
+      <c r="U16" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="V16" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W16" s="15" t="n">
+      <c r="V16" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W16" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X16" s="16" t="n">
+      <c r="X16" s="17" t="n">
         <v>40</v>
       </c>
-      <c r="Y16" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z16" s="13" t="n">
+      <c r="Y16" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z16" s="14" t="n">
         <v>0.2</v>
       </c>
       <c r="AA16" s="9" t="n">
         <f aca="false">(V16/D16)*100</f>
         <v>100</v>
       </c>
-      <c r="AB16" s="13"/>
+      <c r="AB16" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="n">
@@ -1522,59 +1582,63 @@
         <v>0.1392</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="13" t="n">
+      <c r="J17" s="14" t="n">
         <v>102</v>
       </c>
-      <c r="K17" s="13" t="n">
+      <c r="K17" s="14" t="n">
         <v>24</v>
       </c>
       <c r="L17" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M17" s="15" t="n">
+      <c r="M17" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N17" s="16" t="n">
+      <c r="N17" s="17" t="n">
         <v>38.2352</v>
       </c>
       <c r="O17" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P17" s="13" t="n">
+      <c r="P17" s="14" t="n">
         <v>0.2352</v>
       </c>
       <c r="Q17" s="9" t="n">
         <f aca="false">(L17/D17)*100</f>
         <v>100</v>
       </c>
-      <c r="R17" s="9"/>
+      <c r="R17" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S17" s="1"/>
-      <c r="T17" s="13" t="n">
+      <c r="T17" s="14" t="n">
         <v>94</v>
       </c>
-      <c r="U17" s="13" t="n">
+      <c r="U17" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="V17" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W17" s="15" t="n">
+      <c r="V17" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W17" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X17" s="16" t="n">
+      <c r="X17" s="17" t="n">
         <v>39.8936</v>
       </c>
-      <c r="Y17" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z17" s="13" t="n">
+      <c r="Y17" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z17" s="14" t="n">
         <v>0.2021</v>
       </c>
       <c r="AA17" s="9" t="n">
         <f aca="false">(V17/D17)*100</f>
         <v>100</v>
       </c>
-      <c r="AB17" s="13"/>
+      <c r="AB17" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="n">
@@ -1602,59 +1666,63 @@
         <v>0.1315</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="13" t="n">
+      <c r="J18" s="14" t="n">
         <v>93</v>
       </c>
-      <c r="K18" s="13" t="n">
+      <c r="K18" s="14" t="n">
         <v>19</v>
       </c>
       <c r="L18" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M18" s="15" t="n">
+      <c r="M18" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N18" s="16" t="n">
+      <c r="N18" s="17" t="n">
         <v>39.7849</v>
       </c>
       <c r="O18" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P18" s="13" t="n">
+      <c r="P18" s="14" t="n">
         <v>0.2043</v>
       </c>
       <c r="Q18" s="9" t="n">
         <f aca="false">(L18/D18)*100</f>
         <v>100</v>
       </c>
-      <c r="R18" s="9"/>
+      <c r="R18" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S18" s="1"/>
-      <c r="T18" s="13" t="n">
+      <c r="T18" s="14" t="n">
         <v>94</v>
       </c>
-      <c r="U18" s="13" t="n">
+      <c r="U18" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="V18" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W18" s="15" t="n">
+      <c r="V18" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W18" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X18" s="16" t="n">
+      <c r="X18" s="17" t="n">
         <v>41.4893</v>
       </c>
-      <c r="Y18" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z18" s="13" t="n">
+      <c r="Y18" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z18" s="14" t="n">
         <v>0.1702</v>
       </c>
       <c r="AA18" s="9" t="n">
         <f aca="false">(V18/D18)*100</f>
         <v>100</v>
       </c>
-      <c r="AB18" s="13"/>
+      <c r="AB18" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="n">
@@ -1682,59 +1750,63 @@
         <v>0.178</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="13" t="n">
+      <c r="J19" s="14" t="n">
         <v>78</v>
       </c>
-      <c r="K19" s="13" t="n">
+      <c r="K19" s="14" t="n">
         <v>10</v>
       </c>
       <c r="L19" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M19" s="15" t="n">
+      <c r="M19" s="16" t="n">
         <v>28</v>
       </c>
-      <c r="N19" s="16" t="n">
+      <c r="N19" s="17" t="n">
         <v>43.5897</v>
       </c>
       <c r="O19" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P19" s="13" t="n">
+      <c r="P19" s="14" t="n">
         <v>0.1282</v>
       </c>
       <c r="Q19" s="9" t="n">
         <f aca="false">(L19/D19)*100</f>
         <v>100</v>
       </c>
-      <c r="R19" s="9"/>
+      <c r="R19" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S19" s="1"/>
-      <c r="T19" s="13" t="n">
+      <c r="T19" s="14" t="n">
         <v>89</v>
       </c>
-      <c r="U19" s="13" t="n">
+      <c r="U19" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="V19" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W19" s="15" t="n">
+      <c r="V19" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W19" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X19" s="16" t="n">
+      <c r="X19" s="17" t="n">
         <v>40.4494</v>
       </c>
-      <c r="Y19" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z19" s="13" t="n">
+      <c r="Y19" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z19" s="14" t="n">
         <v>0.191</v>
       </c>
       <c r="AA19" s="9" t="n">
         <f aca="false">(V19/D19)*100</f>
         <v>100</v>
       </c>
-      <c r="AB19" s="13"/>
+      <c r="AB19" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
@@ -1762,59 +1834,63 @@
         <v>0.1688</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="13" t="n">
+      <c r="J20" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="K20" s="13" t="n">
+      <c r="K20" s="14" t="n">
         <v>13</v>
       </c>
       <c r="L20" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M20" s="15" t="n">
+      <c r="M20" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N20" s="16" t="n">
+      <c r="N20" s="17" t="n">
         <v>42.9347</v>
       </c>
       <c r="O20" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P20" s="13" t="n">
+      <c r="P20" s="14" t="n">
         <v>0.1413</v>
       </c>
       <c r="Q20" s="9" t="n">
         <f aca="false">(L20/D20)*100</f>
         <v>100</v>
       </c>
-      <c r="R20" s="9"/>
+      <c r="R20" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S20" s="1"/>
-      <c r="T20" s="13" t="n">
+      <c r="T20" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U20" s="13" t="n">
+      <c r="U20" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="V20" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W20" s="15" t="n">
+      <c r="V20" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W20" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X20" s="16" t="n">
+      <c r="X20" s="17" t="n">
         <v>40.7608</v>
       </c>
-      <c r="Y20" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z20" s="13" t="n">
+      <c r="Y20" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z20" s="14" t="n">
         <v>0.1847</v>
       </c>
       <c r="AA20" s="9" t="n">
         <f aca="false">(V20/D20)*100</f>
         <v>100</v>
       </c>
-      <c r="AB20" s="13"/>
+      <c r="AB20" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
@@ -1842,59 +1918,63 @@
         <v>0.1126</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="13" t="n">
+      <c r="J21" s="14" t="n">
         <v>98</v>
       </c>
-      <c r="K21" s="13" t="n">
+      <c r="K21" s="14" t="n">
         <v>19</v>
       </c>
       <c r="L21" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M21" s="15" t="n">
+      <c r="M21" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N21" s="16" t="n">
+      <c r="N21" s="17" t="n">
         <v>40.3061</v>
       </c>
       <c r="O21" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P21" s="13" t="n">
+      <c r="P21" s="14" t="n">
         <v>0.1938</v>
       </c>
       <c r="Q21" s="9" t="n">
         <f aca="false">(L21/D21)*100</f>
         <v>100</v>
       </c>
-      <c r="R21" s="9"/>
+      <c r="R21" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S21" s="1"/>
-      <c r="T21" s="13" t="n">
+      <c r="T21" s="14" t="n">
         <v>90</v>
       </c>
-      <c r="U21" s="13" t="n">
+      <c r="U21" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="V21" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W21" s="15" t="n">
+      <c r="V21" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W21" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X21" s="16" t="n">
+      <c r="X21" s="17" t="n">
         <v>40.5555</v>
       </c>
-      <c r="Y21" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z21" s="13" t="n">
+      <c r="Y21" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z21" s="14" t="n">
         <v>0.1888</v>
       </c>
       <c r="AA21" s="9" t="n">
         <f aca="false">(V21/D21)*100</f>
         <v>100</v>
       </c>
-      <c r="AB21" s="13"/>
+      <c r="AB21" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
@@ -1922,59 +2002,63 @@
         <v>0.1285</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="13" t="n">
+      <c r="J22" s="14" t="n">
         <v>88</v>
       </c>
-      <c r="K22" s="13" t="n">
+      <c r="K22" s="14" t="n">
         <v>14</v>
       </c>
       <c r="L22" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M22" s="15" t="n">
+      <c r="M22" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N22" s="16" t="n">
+      <c r="N22" s="17" t="n">
         <v>42.0454</v>
       </c>
       <c r="O22" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P22" s="13" t="n">
+      <c r="P22" s="14" t="n">
         <v>0.159</v>
       </c>
       <c r="Q22" s="9" t="n">
         <f aca="false">(L22/D22)*100</f>
         <v>100</v>
       </c>
-      <c r="R22" s="9"/>
+      <c r="R22" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S22" s="1"/>
-      <c r="T22" s="13" t="n">
+      <c r="T22" s="14" t="n">
         <v>88</v>
       </c>
-      <c r="U22" s="13" t="n">
+      <c r="U22" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="V22" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W22" s="15" t="n">
+      <c r="V22" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W22" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X22" s="16" t="n">
+      <c r="X22" s="17" t="n">
         <v>40.909</v>
       </c>
-      <c r="Y22" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z22" s="13" t="n">
+      <c r="Y22" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z22" s="14" t="n">
         <v>0.1818</v>
       </c>
       <c r="AA22" s="9" t="n">
         <f aca="false">(V22/D22)*100</f>
         <v>100</v>
       </c>
-      <c r="AB22" s="13"/>
+      <c r="AB22" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
@@ -2002,59 +2086,63 @@
         <v>0.1733</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="13" t="n">
+      <c r="J23" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="K23" s="13" t="n">
+      <c r="K23" s="14" t="n">
         <v>21</v>
       </c>
       <c r="L23" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M23" s="15" t="n">
+      <c r="M23" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N23" s="16" t="n">
+      <c r="N23" s="17" t="n">
         <v>38.5869</v>
       </c>
       <c r="O23" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P23" s="13" t="n">
+      <c r="P23" s="14" t="n">
         <v>0.2282</v>
       </c>
       <c r="Q23" s="9" t="n">
         <f aca="false">(L23/D23)*100</f>
         <v>100</v>
       </c>
-      <c r="R23" s="9"/>
+      <c r="R23" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S23" s="1"/>
-      <c r="T23" s="13" t="n">
+      <c r="T23" s="14" t="n">
         <v>90</v>
       </c>
-      <c r="U23" s="13" t="n">
+      <c r="U23" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="V23" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W23" s="15" t="n">
+      <c r="V23" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W23" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X23" s="16" t="n">
+      <c r="X23" s="17" t="n">
         <v>41.1111</v>
       </c>
-      <c r="Y23" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z23" s="13" t="n">
+      <c r="Y23" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z23" s="14" t="n">
         <v>0.1777</v>
       </c>
       <c r="AA23" s="9" t="n">
         <f aca="false">(V23/D23)*100</f>
         <v>100</v>
       </c>
-      <c r="AB23" s="13"/>
+      <c r="AB23" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="n">
@@ -2082,59 +2170,63 @@
         <v>0.1842</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="13" t="n">
+      <c r="J24" s="14" t="n">
         <v>91</v>
       </c>
-      <c r="K24" s="13" t="n">
+      <c r="K24" s="14" t="n">
         <v>14</v>
       </c>
       <c r="L24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M24" s="15" t="n">
+      <c r="M24" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N24" s="16" t="n">
+      <c r="N24" s="17" t="n">
         <v>42.3076</v>
       </c>
       <c r="O24" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P24" s="13" t="n">
+      <c r="P24" s="14" t="n">
         <v>0.1538</v>
       </c>
       <c r="Q24" s="9" t="n">
         <f aca="false">(L24/D24)*100</f>
         <v>100</v>
       </c>
-      <c r="R24" s="9"/>
+      <c r="R24" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S24" s="1"/>
-      <c r="T24" s="13" t="n">
+      <c r="T24" s="14" t="n">
         <v>103</v>
       </c>
-      <c r="U24" s="13" t="n">
+      <c r="U24" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="V24" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W24" s="15" t="n">
+      <c r="V24" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W24" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X24" s="16" t="n">
+      <c r="X24" s="17" t="n">
         <v>39.8058</v>
       </c>
-      <c r="Y24" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z24" s="13" t="n">
+      <c r="Y24" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z24" s="14" t="n">
         <v>0.2038</v>
       </c>
       <c r="AA24" s="9" t="n">
         <f aca="false">(V24/D24)*100</f>
         <v>100</v>
       </c>
-      <c r="AB24" s="13"/>
+      <c r="AB24" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="n">
@@ -2162,59 +2254,63 @@
         <v>0.2428</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="13" t="n">
+      <c r="J25" s="14" t="n">
         <v>101</v>
       </c>
-      <c r="K25" s="13" t="n">
+      <c r="K25" s="14" t="n">
         <v>21</v>
       </c>
       <c r="L25" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M25" s="15" t="n">
+      <c r="M25" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N25" s="16" t="n">
+      <c r="N25" s="17" t="n">
         <v>39.6039</v>
       </c>
       <c r="O25" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P25" s="13" t="n">
+      <c r="P25" s="14" t="n">
         <v>0.2079</v>
       </c>
       <c r="Q25" s="9" t="n">
         <f aca="false">(L25/D25)*100</f>
         <v>100</v>
       </c>
-      <c r="R25" s="9"/>
+      <c r="R25" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S25" s="1"/>
-      <c r="T25" s="13" t="n">
+      <c r="T25" s="14" t="n">
         <v>105</v>
       </c>
-      <c r="U25" s="13" t="n">
+      <c r="U25" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="V25" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W25" s="15" t="n">
+      <c r="V25" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W25" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X25" s="16" t="n">
+      <c r="X25" s="17" t="n">
         <v>38.0952</v>
       </c>
-      <c r="Y25" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z25" s="13" t="n">
+      <c r="Y25" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z25" s="14" t="n">
         <v>0.238</v>
       </c>
       <c r="AA25" s="9" t="n">
         <f aca="false">(V25/D25)*100</f>
         <v>100</v>
       </c>
-      <c r="AB25" s="13"/>
+      <c r="AB25" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="n">
@@ -2242,59 +2338,63 @@
         <v>0.1265</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="13" t="n">
+      <c r="J26" s="14" t="n">
         <v>90</v>
       </c>
-      <c r="K26" s="13" t="n">
+      <c r="K26" s="14" t="n">
         <v>13</v>
       </c>
       <c r="L26" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M26" s="15" t="n">
+      <c r="M26" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N26" s="16" t="n">
+      <c r="N26" s="17" t="n">
         <v>42.7777</v>
       </c>
       <c r="O26" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P26" s="13" t="n">
+      <c r="P26" s="14" t="n">
         <v>0.1444</v>
       </c>
       <c r="Q26" s="9" t="n">
         <f aca="false">(L26/D26)*100</f>
         <v>100</v>
       </c>
-      <c r="R26" s="9"/>
+      <c r="R26" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S26" s="1"/>
-      <c r="T26" s="13" t="n">
+      <c r="T26" s="14" t="n">
         <v>105</v>
       </c>
-      <c r="U26" s="13" t="n">
+      <c r="U26" s="14" t="n">
         <v>27</v>
       </c>
-      <c r="V26" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W26" s="15" t="n">
+      <c r="V26" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W26" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X26" s="16" t="n">
+      <c r="X26" s="17" t="n">
         <v>37.1428</v>
       </c>
-      <c r="Y26" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z26" s="13" t="n">
+      <c r="Y26" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z26" s="14" t="n">
         <v>0.2571</v>
       </c>
       <c r="AA26" s="9" t="n">
         <f aca="false">(V26/D26)*100</f>
         <v>100</v>
       </c>
-      <c r="AB26" s="13"/>
+      <c r="AB26" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="n">
@@ -2322,59 +2422,63 @@
         <v>0.1857</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="J27" s="13" t="n">
+      <c r="J27" s="14" t="n">
         <v>97</v>
       </c>
-      <c r="K27" s="13" t="n">
+      <c r="K27" s="14" t="n">
         <v>16</v>
       </c>
       <c r="L27" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M27" s="15" t="n">
+      <c r="M27" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N27" s="16" t="n">
+      <c r="N27" s="17" t="n">
         <v>41.7525</v>
       </c>
       <c r="O27" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P27" s="13" t="n">
+      <c r="P27" s="14" t="n">
         <v>0.1649</v>
       </c>
       <c r="Q27" s="9" t="n">
         <f aca="false">(L27/D27)*100</f>
         <v>100</v>
       </c>
-      <c r="R27" s="9"/>
+      <c r="R27" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S27" s="1"/>
-      <c r="T27" s="13" t="n">
+      <c r="T27" s="14" t="n">
         <v>87</v>
       </c>
-      <c r="U27" s="13" t="n">
+      <c r="U27" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="V27" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W27" s="15" t="n">
+      <c r="V27" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W27" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X27" s="16" t="n">
+      <c r="X27" s="17" t="n">
         <v>43.1034</v>
       </c>
-      <c r="Y27" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z27" s="13" t="n">
+      <c r="Y27" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z27" s="14" t="n">
         <v>0.1379</v>
       </c>
       <c r="AA27" s="9" t="n">
         <f aca="false">(V27/D27)*100</f>
         <v>100</v>
       </c>
-      <c r="AB27" s="13"/>
+      <c r="AB27" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="n">
@@ -2402,59 +2506,63 @@
         <v>0.1688</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="13" t="n">
+      <c r="J28" s="14" t="n">
         <v>85</v>
       </c>
-      <c r="K28" s="13" t="n">
+      <c r="K28" s="14" t="n">
         <v>11</v>
       </c>
       <c r="L28" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M28" s="15" t="n">
+      <c r="M28" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N28" s="16" t="n">
+      <c r="N28" s="17" t="n">
         <v>43.5294</v>
       </c>
       <c r="O28" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P28" s="13" t="n">
+      <c r="P28" s="14" t="n">
         <v>0.1294</v>
       </c>
       <c r="Q28" s="9" t="n">
         <f aca="false">(L28/D28)*100</f>
         <v>100</v>
       </c>
-      <c r="R28" s="9"/>
+      <c r="R28" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S28" s="1"/>
-      <c r="T28" s="13" t="n">
+      <c r="T28" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U28" s="13" t="n">
+      <c r="U28" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="V28" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W28" s="15" t="n">
+      <c r="V28" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W28" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X28" s="16" t="n">
+      <c r="X28" s="17" t="n">
         <v>38.5869</v>
       </c>
-      <c r="Y28" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z28" s="13" t="n">
+      <c r="Y28" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z28" s="14" t="n">
         <v>0.2282</v>
       </c>
       <c r="AA28" s="9" t="n">
         <f aca="false">(V28/D28)*100</f>
         <v>100</v>
       </c>
-      <c r="AB28" s="13"/>
+      <c r="AB28" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="n">
@@ -2482,59 +2590,63 @@
         <v>0.2179</v>
       </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="13" t="n">
+      <c r="J29" s="14" t="n">
         <v>89</v>
       </c>
-      <c r="K29" s="13" t="n">
+      <c r="K29" s="14" t="n">
         <v>17</v>
       </c>
       <c r="L29" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M29" s="15" t="n">
+      <c r="M29" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N29" s="16" t="n">
+      <c r="N29" s="17" t="n">
         <v>40.4494</v>
       </c>
       <c r="O29" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P29" s="13" t="n">
+      <c r="P29" s="14" t="n">
         <v>0.191</v>
       </c>
       <c r="Q29" s="9" t="n">
         <f aca="false">(L29/D29)*100</f>
         <v>100</v>
       </c>
-      <c r="R29" s="9"/>
+      <c r="R29" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S29" s="1"/>
-      <c r="T29" s="13" t="n">
+      <c r="T29" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U29" s="13" t="n">
+      <c r="U29" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="V29" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W29" s="15" t="n">
+      <c r="V29" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W29" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X29" s="16" t="n">
+      <c r="X29" s="17" t="n">
         <v>40.2173</v>
       </c>
-      <c r="Y29" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z29" s="13" t="n">
+      <c r="Y29" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z29" s="14" t="n">
         <v>0.1956</v>
       </c>
       <c r="AA29" s="9" t="n">
         <f aca="false">(V29/D29)*100</f>
         <v>100</v>
       </c>
-      <c r="AB29" s="13"/>
+      <c r="AB29" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="n">
@@ -2562,59 +2674,63 @@
         <v>0.1604</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="13" t="n">
+      <c r="J30" s="14" t="n">
         <v>96</v>
       </c>
-      <c r="K30" s="13" t="n">
+      <c r="K30" s="14" t="n">
         <v>19</v>
       </c>
       <c r="L30" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M30" s="15" t="n">
+      <c r="M30" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N30" s="16" t="n">
+      <c r="N30" s="17" t="n">
         <v>40.1041</v>
       </c>
       <c r="O30" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P30" s="13" t="n">
+      <c r="P30" s="14" t="n">
         <v>0.1979</v>
       </c>
       <c r="Q30" s="9" t="n">
         <f aca="false">(L30/D30)*100</f>
         <v>100</v>
       </c>
-      <c r="R30" s="9"/>
+      <c r="R30" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S30" s="1"/>
-      <c r="T30" s="13" t="n">
+      <c r="T30" s="14" t="n">
         <v>87</v>
       </c>
-      <c r="U30" s="13" t="n">
+      <c r="U30" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="V30" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W30" s="15" t="n">
+      <c r="V30" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W30" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="X30" s="16" t="n">
+      <c r="X30" s="17" t="n">
         <v>43.6781</v>
       </c>
-      <c r="Y30" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z30" s="13" t="n">
+      <c r="Y30" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z30" s="14" t="n">
         <v>0.1264</v>
       </c>
       <c r="AA30" s="9" t="n">
         <f aca="false">(V30/D30)*100</f>
         <v>100</v>
       </c>
-      <c r="AB30" s="13"/>
+      <c r="AB30" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="n">
@@ -2642,59 +2758,63 @@
         <v>0.1506</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="13" t="n">
+      <c r="J31" s="14" t="n">
         <v>91</v>
       </c>
-      <c r="K31" s="13" t="n">
+      <c r="K31" s="14" t="n">
         <v>15</v>
       </c>
       <c r="L31" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M31" s="15" t="n">
+      <c r="M31" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N31" s="16" t="n">
+      <c r="N31" s="17" t="n">
         <v>41.7582</v>
       </c>
       <c r="O31" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P31" s="13" t="n">
+      <c r="P31" s="14" t="n">
         <v>0.1648</v>
       </c>
       <c r="Q31" s="9" t="n">
         <f aca="false">(L31/D31)*100</f>
         <v>100</v>
       </c>
-      <c r="R31" s="9"/>
+      <c r="R31" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S31" s="1"/>
-      <c r="T31" s="13" t="n">
+      <c r="T31" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U31" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="V31" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W31" s="15" t="n">
+      <c r="U31" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="V31" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W31" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X31" s="16" t="n">
+      <c r="X31" s="17" t="n">
         <v>39.1304</v>
       </c>
-      <c r="Y31" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z31" s="13" t="n">
+      <c r="Y31" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z31" s="14" t="n">
         <v>0.2173</v>
       </c>
       <c r="AA31" s="9" t="n">
         <f aca="false">(V31/D31)*100</f>
         <v>100</v>
       </c>
-      <c r="AB31" s="13"/>
+      <c r="AB31" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="n">
@@ -2722,59 +2842,63 @@
         <v>0.1805</v>
       </c>
       <c r="I32" s="1"/>
-      <c r="J32" s="13" t="n">
+      <c r="J32" s="14" t="n">
         <v>104</v>
       </c>
-      <c r="K32" s="13" t="n">
+      <c r="K32" s="14" t="n">
         <v>28</v>
       </c>
       <c r="L32" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M32" s="15" t="n">
+      <c r="M32" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="N32" s="16" t="n">
+      <c r="N32" s="17" t="n">
         <v>36.5384</v>
       </c>
       <c r="O32" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P32" s="13" t="n">
+      <c r="P32" s="14" t="n">
         <v>0.2692</v>
       </c>
       <c r="Q32" s="9" t="n">
         <f aca="false">(L32/D32)*100</f>
         <v>100</v>
       </c>
-      <c r="R32" s="9"/>
+      <c r="R32" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="S32" s="1"/>
-      <c r="T32" s="13" t="n">
+      <c r="T32" s="14" t="n">
         <v>92</v>
       </c>
-      <c r="U32" s="13" t="n">
+      <c r="U32" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="V32" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W32" s="15" t="n">
+      <c r="V32" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W32" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="X32" s="16" t="n">
+      <c r="X32" s="17" t="n">
         <v>41.8478</v>
       </c>
-      <c r="Y32" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z32" s="13" t="n">
+      <c r="Y32" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z32" s="14" t="n">
         <v>0.163</v>
       </c>
       <c r="AA32" s="9" t="n">
         <f aca="false">(V32/D32)*100</f>
         <v>100</v>
       </c>
-      <c r="AB32" s="13"/>
+      <c r="AB32" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="n">
@@ -2802,63 +2926,67 @@
         <v>0.2375</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="13" t="n">
+      <c r="J33" s="14" t="n">
         <v>97</v>
       </c>
-      <c r="K33" s="13" t="n">
+      <c r="K33" s="14" t="n">
         <v>22</v>
       </c>
       <c r="L33" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M33" s="15" t="n">
+      <c r="M33" s="16" t="n">
         <v>12.5</v>
       </c>
-      <c r="N33" s="16" t="n">
+      <c r="N33" s="17" t="n">
         <v>38.6597</v>
       </c>
       <c r="O33" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="P33" s="13" t="n">
+      <c r="P33" s="14" t="n">
         <v>0.2268</v>
       </c>
       <c r="Q33" s="9" t="n">
         <f aca="false">(L33/D33)*100</f>
         <v>100</v>
       </c>
-      <c r="R33" s="9"/>
+      <c r="R33" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="S33" s="1"/>
-      <c r="T33" s="13" t="n">
+      <c r="T33" s="14" t="n">
         <v>83</v>
       </c>
-      <c r="U33" s="13" t="n">
+      <c r="U33" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="V33" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="W33" s="15" t="n">
+      <c r="V33" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="W33" s="16" t="n">
         <v>14</v>
       </c>
-      <c r="X33" s="16" t="n">
+      <c r="X33" s="17" t="n">
         <v>43.3734</v>
       </c>
-      <c r="Y33" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z33" s="13" t="n">
+      <c r="Y33" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z33" s="14" t="n">
         <v>0.1325</v>
       </c>
       <c r="AA33" s="9" t="n">
         <f aca="false">(V33/D33)*100</f>
         <v>100</v>
       </c>
-      <c r="AB33" s="13"/>
+      <c r="AB33" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B34" s="4" t="n">
         <f aca="false">SUM(B4:B33)</f>
@@ -2868,27 +2996,27 @@
         <f aca="false">SUM(C4:C33)</f>
         <v>391</v>
       </c>
-      <c r="D34" s="18" t="n">
+      <c r="D34" s="19" t="n">
         <f aca="false">SUM(D4:D33)</f>
         <v>600</v>
       </c>
-      <c r="E34" s="19" t="n">
+      <c r="E34" s="20" t="n">
         <f aca="false">SUM(E4:E33)</f>
         <v>562.5</v>
       </c>
-      <c r="F34" s="20" t="n">
+      <c r="F34" s="21" t="n">
         <f aca="false">SUM(F4:F33)</f>
         <v>1237.2269</v>
       </c>
-      <c r="G34" s="21" t="n">
+      <c r="G34" s="22" t="n">
         <f aca="false">SUM(G4:G33)</f>
         <v>1500</v>
       </c>
-      <c r="H34" s="22" t="n">
+      <c r="H34" s="23" t="n">
         <f aca="false">SUM(H4:H33)</f>
         <v>5.2609</v>
       </c>
-      <c r="I34" s="23"/>
+      <c r="I34" s="24"/>
       <c r="J34" s="4" t="n">
         <f aca="false">SUM(J4:J33)</f>
         <v>2791</v>
@@ -2897,23 +3025,23 @@
         <f aca="false">SUM(K4:K33)</f>
         <v>526</v>
       </c>
-      <c r="L34" s="18" t="n">
+      <c r="L34" s="19" t="n">
         <f aca="false">SUM(L4:L33)</f>
         <v>600</v>
       </c>
-      <c r="M34" s="20" t="n">
+      <c r="M34" s="21" t="n">
         <f aca="false">SUM(M4:M33)</f>
         <v>592</v>
       </c>
-      <c r="N34" s="20" t="n">
+      <c r="N34" s="21" t="n">
         <f aca="false">SUM(N4:N33)</f>
         <v>1219.6896</v>
       </c>
-      <c r="O34" s="20" t="n">
+      <c r="O34" s="21" t="n">
         <f aca="false">SUM(O4:O33)</f>
         <v>1500</v>
       </c>
-      <c r="P34" s="22" t="n">
+      <c r="P34" s="23" t="n">
         <f aca="false">SUM(P4:P33)</f>
         <v>5.605</v>
       </c>
@@ -2931,23 +3059,23 @@
         <f aca="false">SUM(U4:U33)</f>
         <v>506</v>
       </c>
-      <c r="V34" s="18" t="n">
+      <c r="V34" s="19" t="n">
         <f aca="false">SUM(V4:V33)</f>
         <v>600</v>
       </c>
-      <c r="W34" s="20" t="n">
+      <c r="W34" s="21" t="n">
         <f aca="false">SUM(W4:W33)</f>
         <v>615.5</v>
       </c>
-      <c r="X34" s="20" t="n">
+      <c r="X34" s="21" t="n">
         <f aca="false">SUM(X4:X33)</f>
         <v>1225.5153</v>
       </c>
-      <c r="Y34" s="20" t="n">
+      <c r="Y34" s="21" t="n">
         <f aca="false">SUM(Y4:Y33)</f>
         <v>1500</v>
       </c>
-      <c r="Z34" s="22" t="n">
+      <c r="Z34" s="23" t="n">
         <f aca="false">SUM(Z4:Z33)</f>
         <v>5.4881</v>
       </c>
@@ -2959,108 +3087,104 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B35" s="20" t="n">
         <f aca="false">B34/30</f>
         <v>74.3666666666667</v>
       </c>
-      <c r="C35" s="18" t="n">
+      <c r="C35" s="19" t="n">
         <f aca="false">C34/30</f>
         <v>13.0333333333333</v>
       </c>
-      <c r="D35" s="18" t="n">
+      <c r="D35" s="19" t="n">
         <f aca="false">D34/30</f>
         <v>20</v>
       </c>
-      <c r="E35" s="24" t="n">
+      <c r="E35" s="25" t="n">
         <f aca="false">E34/30</f>
         <v>18.75</v>
       </c>
-      <c r="F35" s="20" t="n">
+      <c r="F35" s="21" t="n">
         <f aca="false">F34/30</f>
         <v>41.2408966666667</v>
       </c>
-      <c r="G35" s="25" t="n">
+      <c r="G35" s="26" t="n">
         <f aca="false">G34/30</f>
         <v>50</v>
       </c>
-      <c r="H35" s="22" t="n">
+      <c r="H35" s="23" t="n">
         <f aca="false">H34/30</f>
         <v>0.175363333333333</v>
       </c>
-      <c r="I35" s="23"/>
-      <c r="J35" s="19" t="n">
+      <c r="I35" s="24"/>
+      <c r="J35" s="20" t="n">
         <f aca="false">J34/30</f>
         <v>93.0333333333333</v>
       </c>
-      <c r="K35" s="18" t="n">
+      <c r="K35" s="19" t="n">
         <f aca="false">K34/30</f>
         <v>17.5333333333333</v>
       </c>
-      <c r="L35" s="18" t="n">
+      <c r="L35" s="19" t="n">
         <f aca="false">L34/30</f>
         <v>20</v>
       </c>
-      <c r="M35" s="20" t="n">
+      <c r="M35" s="21" t="n">
         <f aca="false">M34/30</f>
         <v>19.7333333333333</v>
       </c>
-      <c r="N35" s="20" t="n">
+      <c r="N35" s="21" t="n">
         <f aca="false">N34/30</f>
         <v>40.65632</v>
       </c>
-      <c r="O35" s="18" t="n">
+      <c r="O35" s="19" t="n">
         <f aca="false">O34/30</f>
         <v>50</v>
       </c>
-      <c r="P35" s="22" t="n">
+      <c r="P35" s="23" t="n">
         <f aca="false">P34/30</f>
         <v>0.186833333333333</v>
       </c>
-      <c r="Q35" s="19" t="n">
+      <c r="Q35" s="20" t="n">
         <f aca="false">Q34/30</f>
         <v>100</v>
       </c>
-      <c r="R35" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="S35" s="27"/>
-      <c r="T35" s="19" t="n">
+      <c r="R35" s="27"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="20" t="n">
         <f aca="false">T34/30</f>
         <v>91.6</v>
       </c>
-      <c r="U35" s="18" t="n">
+      <c r="U35" s="19" t="n">
         <f aca="false">U34/30</f>
         <v>16.8666666666667</v>
       </c>
-      <c r="V35" s="18" t="n">
+      <c r="V35" s="19" t="n">
         <f aca="false">V34/30</f>
         <v>20</v>
       </c>
-      <c r="W35" s="20" t="n">
+      <c r="W35" s="21" t="n">
         <f aca="false">W34/30</f>
         <v>20.5166666666667</v>
       </c>
-      <c r="X35" s="20" t="n">
+      <c r="X35" s="21" t="n">
         <f aca="false">X34/30</f>
         <v>40.85051</v>
       </c>
-      <c r="Y35" s="18" t="n">
+      <c r="Y35" s="19" t="n">
         <f aca="false">Y34/30</f>
         <v>50</v>
       </c>
-      <c r="Z35" s="22" t="n">
+      <c r="Z35" s="23" t="n">
         <f aca="false">Z34/30</f>
         <v>0.182936666666667</v>
       </c>
-      <c r="AA35" s="19" t="n">
+      <c r="AA35" s="20" t="n">
         <f aca="false">AA34/30</f>
         <v>100</v>
       </c>
-      <c r="AB35" s="26" t="s">
-        <v>15</v>
-      </c>
+      <c r="AB35" s="27"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
@@ -3073,7 +3197,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
-      <c r="D39" s="28"/>
+      <c r="D39" s="29"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>

</xml_diff>

<commit_message>
Change headers of the report
</commit_message>
<xml_diff>
--- a/download/Metrics report.xlsx
+++ b/download/Metrics report.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Fails</t>
   </si>
   <si>
-    <t xml:space="preserve">AVG Response Time</t>
+    <t xml:space="preserve">Average response time</t>
   </si>
   <si>
     <t xml:space="preserve">Latency</t>
@@ -49,16 +49,16 @@
     <t xml:space="preserve">Throughput</t>
   </si>
   <si>
-    <t xml:space="preserve">Query Success Rate</t>
+    <t xml:space="preserve">Requisition rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Query Delay</t>
+    <t xml:space="preserve">Drop in the requisition rate</t>
   </si>
   <si>
     <t xml:space="preserve">pLatency</t>
   </si>
   <si>
-    <t xml:space="preserve">Performance Influence Adapt</t>
+    <t xml:space="preserve">Influence of performance on adaptivity (IpA)</t>
   </si>
   <si>
     <t xml:space="preserve">NO</t>
@@ -88,7 +88,7 @@
     <numFmt numFmtId="171" formatCode="0.00%"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -117,6 +117,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -189,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -210,11 +218,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,7 +234,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,19 +258,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,7 +310,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,7 +318,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,18 +341,39 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB4" activeCellId="0" sqref="AB4:AB33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="8" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -404,10 +437,10 @@
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="4" t="s">
         <v>4</v>
       </c>
@@ -432,2555 +465,2555 @@
       <c r="Q3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="8" t="s">
+      <c r="S3" s="8"/>
+      <c r="T3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="Z3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AA3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AB3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="10" t="n">
         <v>82</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E4" s="11" t="n">
+      <c r="D4" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F4" s="12" t="n">
+      <c r="F4" s="13" t="n">
         <v>42.0731</v>
       </c>
-      <c r="G4" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H4" s="9" t="n">
+      <c r="G4" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" s="10" t="n">
         <v>0.1585</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="9" t="n">
+      <c r="J4" s="10" t="n">
         <v>97</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="L4" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M4" s="11" t="n">
+      <c r="L4" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M4" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="N4" s="12" t="n">
+      <c r="N4" s="13" t="n">
         <v>42.268</v>
       </c>
-      <c r="O4" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P4" s="9" t="n">
+      <c r="O4" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P4" s="10" t="n">
         <v>0.1546</v>
       </c>
-      <c r="Q4" s="9" t="n">
+      <c r="Q4" s="10" t="n">
         <f aca="false">(L4/D4)*100</f>
         <v>100</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="14" t="n">
+      <c r="T4" s="15" t="n">
         <v>86</v>
       </c>
-      <c r="U4" s="14" t="n">
+      <c r="U4" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="V4" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W4" s="16" t="n">
+      <c r="V4" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W4" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X4" s="17" t="n">
+      <c r="X4" s="18" t="n">
         <v>39.5348</v>
       </c>
-      <c r="Y4" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z4" s="14" t="n">
+      <c r="Y4" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z4" s="15" t="n">
         <v>0.2093</v>
       </c>
-      <c r="AA4" s="9" t="n">
+      <c r="AA4" s="10" t="n">
         <f aca="false">(V4/D4)*100</f>
         <v>100</v>
       </c>
-      <c r="AB4" s="13" t="s">
+      <c r="AB4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="10" t="n">
         <v>77</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="D5" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" s="11" t="n">
+      <c r="D5" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F5" s="12" t="n">
+      <c r="F5" s="13" t="n">
         <v>38.3116</v>
       </c>
-      <c r="G5" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H5" s="9" t="n">
+      <c r="G5" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H5" s="10" t="n">
         <v>0.2337</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="9" t="n">
+      <c r="J5" s="10" t="n">
         <v>89</v>
       </c>
-      <c r="K5" s="9" t="n">
+      <c r="K5" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="L5" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M5" s="11" t="n">
+      <c r="L5" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M5" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="N5" s="12" t="n">
+      <c r="N5" s="13" t="n">
         <v>39.3258</v>
       </c>
-      <c r="O5" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P5" s="9" t="n">
+      <c r="O5" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P5" s="10" t="n">
         <v>0.2134</v>
       </c>
-      <c r="Q5" s="9" t="n">
+      <c r="Q5" s="10" t="n">
         <f aca="false">(L5/D5)*100</f>
         <v>100</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="14" t="n">
+      <c r="T5" s="15" t="n">
         <v>87</v>
       </c>
-      <c r="U5" s="14" t="n">
+      <c r="U5" s="15" t="n">
         <v>14</v>
       </c>
-      <c r="V5" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W5" s="16" t="n">
+      <c r="V5" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W5" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="X5" s="17" t="n">
+      <c r="X5" s="18" t="n">
         <v>41.954</v>
       </c>
-      <c r="Y5" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z5" s="14" t="n">
+      <c r="Y5" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z5" s="15" t="n">
         <v>0.1609</v>
       </c>
-      <c r="AA5" s="9" t="n">
+      <c r="AA5" s="10" t="n">
         <f aca="false">(V5/D5)*100</f>
         <v>100</v>
       </c>
-      <c r="AB5" s="13" t="s">
+      <c r="AB5" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
+      <c r="A6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <v>71</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="D6" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E6" s="11" t="n">
+      <c r="D6" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F6" s="12" t="n">
+      <c r="F6" s="13" t="n">
         <v>40.1408</v>
       </c>
-      <c r="G6" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H6" s="9" t="n">
+      <c r="G6" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H6" s="10" t="n">
         <v>0.1971</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="10" t="n">
         <v>90</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="L6" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M6" s="11" t="n">
+      <c r="L6" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M6" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N6" s="12" t="n">
+      <c r="N6" s="13" t="n">
         <v>41.1111</v>
       </c>
-      <c r="O6" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P6" s="9" t="n">
+      <c r="O6" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P6" s="10" t="n">
         <v>0.1777</v>
       </c>
-      <c r="Q6" s="9" t="n">
+      <c r="Q6" s="10" t="n">
         <f aca="false">(L6/D6)*100</f>
         <v>100</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="14" t="n">
+      <c r="T6" s="15" t="n">
         <v>89</v>
       </c>
-      <c r="U6" s="14" t="n">
+      <c r="U6" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V6" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W6" s="16" t="n">
+      <c r="V6" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W6" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X6" s="17" t="n">
+      <c r="X6" s="18" t="n">
         <v>41.0112</v>
       </c>
-      <c r="Y6" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z6" s="14" t="n">
+      <c r="Y6" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="15" t="n">
         <v>0.1797</v>
       </c>
-      <c r="AA6" s="9" t="n">
+      <c r="AA6" s="10" t="n">
         <f aca="false">(V6/D6)*100</f>
         <v>100</v>
       </c>
-      <c r="AB6" s="13" t="s">
+      <c r="AB6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
+      <c r="A7" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>69</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="D7" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E7" s="11" t="n">
+      <c r="D7" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F7" s="12" t="n">
+      <c r="F7" s="13" t="n">
         <v>43.4782</v>
       </c>
-      <c r="G7" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H7" s="9" t="n">
+      <c r="G7" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H7" s="10" t="n">
         <v>0.1384</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="9" t="n">
+      <c r="J7" s="10" t="n">
         <v>92</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="L7" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M7" s="11" t="n">
+      <c r="L7" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M7" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N7" s="12" t="n">
+      <c r="N7" s="13" t="n">
         <v>41.3043</v>
       </c>
-      <c r="O7" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P7" s="9" t="n">
+      <c r="O7" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P7" s="10" t="n">
         <v>0.1739</v>
       </c>
-      <c r="Q7" s="9" t="n">
+      <c r="Q7" s="10" t="n">
         <f aca="false">(L7/D7)*100</f>
         <v>100</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S7" s="1"/>
-      <c r="T7" s="14" t="n">
+      <c r="T7" s="15" t="n">
         <v>88</v>
       </c>
-      <c r="U7" s="14" t="n">
+      <c r="U7" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="V7" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W7" s="16" t="n">
+      <c r="V7" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W7" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X7" s="17" t="n">
+      <c r="X7" s="18" t="n">
         <v>40.3409</v>
       </c>
-      <c r="Y7" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z7" s="14" t="n">
+      <c r="Y7" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z7" s="15" t="n">
         <v>0.1931</v>
       </c>
-      <c r="AA7" s="9" t="n">
+      <c r="AA7" s="10" t="n">
         <f aca="false">(V7/D7)*100</f>
         <v>100</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
+      <c r="A8" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="10" t="n">
         <v>74</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="D8" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E8" s="11" t="n">
+      <c r="D8" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F8" s="13" t="n">
         <v>38.5135</v>
       </c>
-      <c r="G8" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H8" s="9" t="n">
+      <c r="G8" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H8" s="10" t="n">
         <v>0.2287</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="9" t="n">
+      <c r="J8" s="10" t="n">
         <v>88</v>
       </c>
-      <c r="K8" s="9" t="n">
+      <c r="K8" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="L8" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M8" s="11" t="n">
+      <c r="L8" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N8" s="12" t="n">
+      <c r="N8" s="13" t="n">
         <v>36.9318</v>
       </c>
-      <c r="O8" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P8" s="9" t="n">
+      <c r="O8" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P8" s="10" t="n">
         <v>0.2613</v>
       </c>
-      <c r="Q8" s="9" t="n">
+      <c r="Q8" s="10" t="n">
         <f aca="false">(L8/D8)*100</f>
         <v>100</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S8" s="1"/>
-      <c r="T8" s="14" t="n">
+      <c r="T8" s="15" t="n">
         <v>98</v>
       </c>
-      <c r="U8" s="14" t="n">
+      <c r="U8" s="15" t="n">
         <v>21</v>
       </c>
-      <c r="V8" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W8" s="16" t="n">
+      <c r="V8" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W8" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X8" s="17" t="n">
+      <c r="X8" s="18" t="n">
         <v>39.2857</v>
       </c>
-      <c r="Y8" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z8" s="14" t="n">
+      <c r="Y8" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z8" s="15" t="n">
         <v>0.2142</v>
       </c>
-      <c r="AA8" s="9" t="n">
+      <c r="AA8" s="10" t="n">
         <f aca="false">(V8/D8)*100</f>
         <v>100</v>
       </c>
-      <c r="AB8" s="13" t="s">
+      <c r="AB8" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D9" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E9" s="11" t="n">
+      <c r="D9" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F9" s="12" t="n">
+      <c r="F9" s="13" t="n">
         <v>42.8571</v>
       </c>
-      <c r="G9" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H9" s="9" t="n">
+      <c r="G9" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H9" s="10" t="n">
         <v>0.1428</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="10" t="n">
         <v>101</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="L9" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M9" s="11" t="n">
+      <c r="L9" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M9" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="N9" s="12" t="n">
+      <c r="N9" s="13" t="n">
         <v>38.1188</v>
       </c>
-      <c r="O9" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P9" s="9" t="n">
+      <c r="O9" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P9" s="10" t="n">
         <v>0.2376</v>
       </c>
-      <c r="Q9" s="9" t="n">
+      <c r="Q9" s="10" t="n">
         <f aca="false">(L9/D9)*100</f>
         <v>100</v>
       </c>
-      <c r="R9" s="13" t="s">
+      <c r="R9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S9" s="1"/>
-      <c r="T9" s="14" t="n">
+      <c r="T9" s="15" t="n">
         <v>91</v>
       </c>
-      <c r="U9" s="14" t="n">
+      <c r="U9" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="V9" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W9" s="16" t="n">
+      <c r="V9" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W9" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X9" s="17" t="n">
+      <c r="X9" s="18" t="n">
         <v>39.5604</v>
       </c>
-      <c r="Y9" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z9" s="14" t="n">
+      <c r="Y9" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="15" t="n">
         <v>0.2087</v>
       </c>
-      <c r="AA9" s="9" t="n">
+      <c r="AA9" s="10" t="n">
         <f aca="false">(V9/D9)*100</f>
         <v>100</v>
       </c>
-      <c r="AB9" s="13" t="s">
+      <c r="AB9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="n">
+      <c r="A10" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D10" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E10" s="11" t="n">
+      <c r="D10" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F10" s="12" t="n">
+      <c r="F10" s="13" t="n">
         <v>40.7142</v>
       </c>
-      <c r="G10" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H10" s="9" t="n">
+      <c r="G10" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H10" s="10" t="n">
         <v>0.1857</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="K10" s="9" t="n">
+      <c r="J10" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="K10" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="L10" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M10" s="11" t="n">
+      <c r="L10" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M10" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N10" s="12" t="n">
+      <c r="N10" s="13" t="n">
         <v>38.5</v>
       </c>
-      <c r="O10" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P10" s="9" t="n">
+      <c r="O10" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P10" s="10" t="n">
         <v>0.23</v>
       </c>
-      <c r="Q10" s="9" t="n">
+      <c r="Q10" s="10" t="n">
         <f aca="false">(L10/D10)*100</f>
         <v>100</v>
       </c>
-      <c r="R10" s="13" t="s">
+      <c r="R10" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S10" s="1"/>
-      <c r="T10" s="14" t="n">
+      <c r="T10" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U10" s="14" t="n">
+      <c r="U10" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V10" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W10" s="16" t="n">
+      <c r="V10" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W10" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X10" s="17" t="n">
+      <c r="X10" s="18" t="n">
         <v>41.3043</v>
       </c>
-      <c r="Y10" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z10" s="14" t="n">
+      <c r="Y10" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z10" s="15" t="n">
         <v>0.1739</v>
       </c>
-      <c r="AA10" s="9" t="n">
+      <c r="AA10" s="10" t="n">
         <f aca="false">(V10/D10)*100</f>
         <v>100</v>
       </c>
-      <c r="AB10" s="13" t="s">
+      <c r="AB10" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
+      <c r="A11" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="10" t="n">
         <v>76</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D11" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E11" s="11" t="n">
+      <c r="D11" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" s="13" t="n">
         <v>41.4473</v>
       </c>
-      <c r="G11" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H11" s="9" t="n">
+      <c r="G11" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H11" s="10" t="n">
         <v>0.171</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="9" t="n">
+      <c r="J11" s="10" t="n">
         <v>101</v>
       </c>
-      <c r="K11" s="9" t="n">
+      <c r="K11" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="L11" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M11" s="11" t="n">
+      <c r="L11" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M11" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="N11" s="12" t="n">
+      <c r="N11" s="13" t="n">
         <v>39.1089</v>
       </c>
-      <c r="O11" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P11" s="9" t="n">
+      <c r="O11" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P11" s="10" t="n">
         <v>0.2178</v>
       </c>
-      <c r="Q11" s="9" t="n">
+      <c r="Q11" s="10" t="n">
         <f aca="false">(L11/D11)*100</f>
         <v>100</v>
       </c>
-      <c r="R11" s="13" t="s">
+      <c r="R11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="1"/>
-      <c r="T11" s="14" t="n">
+      <c r="T11" s="15" t="n">
         <v>90</v>
       </c>
-      <c r="U11" s="14" t="n">
+      <c r="U11" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="V11" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W11" s="16" t="n">
+      <c r="V11" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W11" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X11" s="17" t="n">
+      <c r="X11" s="18" t="n">
         <v>44.4444</v>
       </c>
-      <c r="Y11" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z11" s="14" t="n">
+      <c r="Y11" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z11" s="15" t="n">
         <v>0.1111</v>
       </c>
-      <c r="AA11" s="9" t="n">
+      <c r="AA11" s="10" t="n">
         <f aca="false">(V11/D11)*100</f>
         <v>100</v>
       </c>
-      <c r="AB11" s="13" t="s">
+      <c r="AB11" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="n">
+      <c r="A12" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <v>72</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="D12" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E12" s="11" t="n">
+      <c r="D12" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E12" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F12" s="18" t="n">
+      <c r="F12" s="19" t="n">
         <v>43.75</v>
       </c>
-      <c r="G12" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H12" s="9" t="n">
+      <c r="G12" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H12" s="10" t="n">
         <v>0.125</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="9" t="n">
+      <c r="J12" s="10" t="n">
         <v>92</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="L12" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M12" s="11" t="n">
+      <c r="L12" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M12" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N12" s="18" t="n">
+      <c r="N12" s="19" t="n">
         <v>41.8478</v>
       </c>
-      <c r="O12" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P12" s="9" t="n">
+      <c r="O12" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P12" s="10" t="n">
         <v>0.163</v>
       </c>
-      <c r="Q12" s="9" t="n">
+      <c r="Q12" s="10" t="n">
         <f aca="false">(L12/D12)*100</f>
         <v>100</v>
       </c>
-      <c r="R12" s="13" t="s">
+      <c r="R12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S12" s="1"/>
-      <c r="T12" s="14" t="n">
+      <c r="T12" s="15" t="n">
         <v>91</v>
       </c>
-      <c r="U12" s="14" t="n">
+      <c r="U12" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="V12" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W12" s="16" t="n">
+      <c r="V12" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W12" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X12" s="17" t="n">
+      <c r="X12" s="18" t="n">
         <v>44.5054</v>
       </c>
-      <c r="Y12" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z12" s="14" t="n">
+      <c r="Y12" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z12" s="15" t="n">
         <v>0.1098</v>
       </c>
-      <c r="AA12" s="9" t="n">
+      <c r="AA12" s="10" t="n">
         <f aca="false">(V12/D12)*100</f>
         <v>100</v>
       </c>
-      <c r="AB12" s="13" t="s">
+      <c r="AB12" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="n">
+      <c r="A13" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="D13" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E13" s="11" t="n">
+      <c r="D13" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F13" s="12" t="n">
+      <c r="F13" s="13" t="n">
         <v>39.2857</v>
       </c>
-      <c r="G13" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H13" s="9" t="n">
+      <c r="G13" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H13" s="10" t="n">
         <v>0.2142</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="9" t="n">
+      <c r="J13" s="10" t="n">
         <v>88</v>
       </c>
-      <c r="K13" s="9" t="n">
+      <c r="K13" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="L13" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M13" s="11" t="n">
+      <c r="L13" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M13" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N13" s="12" t="n">
+      <c r="N13" s="13" t="n">
         <v>42.0454</v>
       </c>
-      <c r="O13" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P13" s="9" t="n">
+      <c r="O13" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P13" s="10" t="n">
         <v>0.159</v>
       </c>
-      <c r="Q13" s="9" t="n">
+      <c r="Q13" s="10" t="n">
         <f aca="false">(L13/D13)*100</f>
         <v>100</v>
       </c>
-      <c r="R13" s="13" t="s">
+      <c r="R13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S13" s="1"/>
-      <c r="T13" s="14" t="n">
+      <c r="T13" s="15" t="n">
         <v>95</v>
       </c>
-      <c r="U13" s="14" t="n">
+      <c r="U13" s="15" t="n">
         <v>15</v>
       </c>
-      <c r="V13" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W13" s="16" t="n">
+      <c r="V13" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W13" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X13" s="17" t="n">
+      <c r="X13" s="18" t="n">
         <v>42.1875</v>
       </c>
-      <c r="Y13" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z13" s="14" t="n">
+      <c r="Y13" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z13" s="15" t="n">
         <v>0.1562</v>
       </c>
-      <c r="AA13" s="9" t="n">
+      <c r="AA13" s="10" t="n">
         <f aca="false">(V13/D13)*100</f>
         <v>100</v>
       </c>
-      <c r="AB13" s="13" t="s">
+      <c r="AB13" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="n">
+      <c r="A14" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="10" t="n">
         <v>75</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E14" s="11" t="n">
+      <c r="D14" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F14" s="12" t="n">
+      <c r="F14" s="13" t="n">
         <v>43.3333</v>
       </c>
-      <c r="G14" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H14" s="9" t="n">
+      <c r="G14" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H14" s="10" t="n">
         <v>0.1333</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="9" t="n">
+      <c r="J14" s="10" t="n">
         <v>99</v>
       </c>
-      <c r="K14" s="9" t="n">
+      <c r="K14" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="L14" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M14" s="11" t="n">
+      <c r="L14" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M14" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="N14" s="12" t="n">
+      <c r="N14" s="13" t="n">
         <v>40.909</v>
       </c>
-      <c r="O14" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P14" s="9" t="n">
+      <c r="O14" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P14" s="10" t="n">
         <v>0.1818</v>
       </c>
-      <c r="Q14" s="9" t="n">
+      <c r="Q14" s="10" t="n">
         <f aca="false">(L14/D14)*100</f>
         <v>100</v>
       </c>
-      <c r="R14" s="13" t="s">
+      <c r="R14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S14" s="1"/>
-      <c r="T14" s="14" t="n">
+      <c r="T14" s="15" t="n">
         <v>84</v>
       </c>
-      <c r="U14" s="14" t="n">
+      <c r="U14" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V14" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W14" s="16" t="n">
+      <c r="V14" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W14" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X14" s="17" t="n">
+      <c r="X14" s="18" t="n">
         <v>40.4761</v>
       </c>
-      <c r="Y14" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z14" s="14" t="n">
+      <c r="Y14" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z14" s="15" t="n">
         <v>0.1904</v>
       </c>
-      <c r="AA14" s="9" t="n">
+      <c r="AA14" s="10" t="n">
         <f aca="false">(V14/D14)*100</f>
         <v>100</v>
       </c>
-      <c r="AB14" s="13" t="s">
+      <c r="AB14" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="n">
+      <c r="A15" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="10" t="n">
         <v>73</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="D15" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E15" s="11" t="n">
+      <c r="D15" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F15" s="12" t="n">
+      <c r="F15" s="13" t="n">
         <v>39.041</v>
       </c>
-      <c r="G15" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H15" s="9" t="n">
+      <c r="G15" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H15" s="10" t="n">
         <v>0.2191</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="9" t="n">
+      <c r="J15" s="10" t="n">
         <v>88</v>
       </c>
-      <c r="K15" s="9" t="n">
+      <c r="K15" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="L15" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M15" s="11" t="n">
+      <c r="L15" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M15" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="N15" s="12" t="n">
+      <c r="N15" s="13" t="n">
         <v>43.1818</v>
       </c>
-      <c r="O15" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P15" s="9" t="n">
+      <c r="O15" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P15" s="10" t="n">
         <v>0.1363</v>
       </c>
-      <c r="Q15" s="9" t="n">
+      <c r="Q15" s="10" t="n">
         <f aca="false">(L15/D15)*100</f>
         <v>100</v>
       </c>
-      <c r="R15" s="13" t="s">
+      <c r="R15" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S15" s="1"/>
-      <c r="T15" s="14" t="n">
+      <c r="T15" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U15" s="14" t="n">
+      <c r="U15" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="V15" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W15" s="16" t="n">
+      <c r="V15" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W15" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X15" s="17" t="n">
+      <c r="X15" s="18" t="n">
         <v>40.7608</v>
       </c>
-      <c r="Y15" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z15" s="14" t="n">
+      <c r="Y15" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z15" s="15" t="n">
         <v>0.1847</v>
       </c>
-      <c r="AA15" s="9" t="n">
+      <c r="AA15" s="10" t="n">
         <f aca="false">(V15/D15)*100</f>
         <v>100</v>
       </c>
-      <c r="AB15" s="13" t="s">
+      <c r="AB15" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="n">
+      <c r="A16" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="10" t="n">
         <v>75</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="D16" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E16" s="11" t="n">
+      <c r="D16" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F16" s="12" t="n">
+      <c r="F16" s="13" t="n">
         <v>38.6666</v>
       </c>
-      <c r="G16" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H16" s="9" t="n">
+      <c r="G16" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H16" s="10" t="n">
         <v>0.2266</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="14" t="n">
+      <c r="J16" s="15" t="n">
         <v>82</v>
       </c>
-      <c r="K16" s="14" t="n">
+      <c r="K16" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="L16" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M16" s="16" t="n">
+      <c r="L16" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M16" s="17" t="n">
         <v>26.5</v>
       </c>
-      <c r="N16" s="17" t="n">
+      <c r="N16" s="18" t="n">
         <v>42.0731</v>
       </c>
-      <c r="O16" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P16" s="14" t="n">
+      <c r="O16" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P16" s="15" t="n">
         <v>0.1585</v>
       </c>
-      <c r="Q16" s="9" t="n">
+      <c r="Q16" s="10" t="n">
         <f aca="false">(L16/D16)*100</f>
         <v>100</v>
       </c>
-      <c r="R16" s="13" t="s">
+      <c r="R16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S16" s="1"/>
-      <c r="T16" s="14" t="n">
+      <c r="T16" s="15" t="n">
         <v>90</v>
       </c>
-      <c r="U16" s="14" t="n">
+      <c r="U16" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="V16" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W16" s="16" t="n">
+      <c r="V16" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W16" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X16" s="17" t="n">
+      <c r="X16" s="18" t="n">
         <v>40</v>
       </c>
-      <c r="Y16" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z16" s="14" t="n">
+      <c r="Y16" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z16" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="AA16" s="9" t="n">
+      <c r="AA16" s="10" t="n">
         <f aca="false">(V16/D16)*100</f>
         <v>100</v>
       </c>
-      <c r="AB16" s="13" t="s">
+      <c r="AB16" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="n">
+      <c r="A17" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="10" t="n">
         <v>79</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="D17" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E17" s="11" t="n">
+      <c r="D17" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F17" s="12" t="n">
+      <c r="F17" s="13" t="n">
         <v>43.0379</v>
       </c>
-      <c r="G17" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H17" s="9" t="n">
+      <c r="G17" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H17" s="10" t="n">
         <v>0.1392</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="14" t="n">
+      <c r="J17" s="15" t="n">
         <v>102</v>
       </c>
-      <c r="K17" s="14" t="n">
+      <c r="K17" s="15" t="n">
         <v>24</v>
       </c>
-      <c r="L17" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M17" s="16" t="n">
+      <c r="L17" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M17" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N17" s="17" t="n">
+      <c r="N17" s="18" t="n">
         <v>38.2352</v>
       </c>
-      <c r="O17" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P17" s="14" t="n">
+      <c r="O17" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P17" s="15" t="n">
         <v>0.2352</v>
       </c>
-      <c r="Q17" s="9" t="n">
+      <c r="Q17" s="10" t="n">
         <f aca="false">(L17/D17)*100</f>
         <v>100</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="R17" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S17" s="1"/>
-      <c r="T17" s="14" t="n">
+      <c r="T17" s="15" t="n">
         <v>94</v>
       </c>
-      <c r="U17" s="14" t="n">
+      <c r="U17" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="V17" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W17" s="16" t="n">
+      <c r="V17" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W17" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X17" s="17" t="n">
+      <c r="X17" s="18" t="n">
         <v>39.8936</v>
       </c>
-      <c r="Y17" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z17" s="14" t="n">
+      <c r="Y17" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z17" s="15" t="n">
         <v>0.2021</v>
       </c>
-      <c r="AA17" s="9" t="n">
+      <c r="AA17" s="10" t="n">
         <f aca="false">(V17/D17)*100</f>
         <v>100</v>
       </c>
-      <c r="AB17" s="13" t="s">
+      <c r="AB17" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="n">
+      <c r="A18" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="10" t="n">
         <v>76</v>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D18" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E18" s="11" t="n">
+      <c r="D18" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E18" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F18" s="12" t="n">
+      <c r="F18" s="13" t="n">
         <v>43.421</v>
       </c>
-      <c r="G18" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H18" s="9" t="n">
+      <c r="G18" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H18" s="10" t="n">
         <v>0.1315</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="14" t="n">
+      <c r="J18" s="15" t="n">
         <v>93</v>
       </c>
-      <c r="K18" s="14" t="n">
+      <c r="K18" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="L18" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M18" s="16" t="n">
+      <c r="L18" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M18" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N18" s="17" t="n">
+      <c r="N18" s="18" t="n">
         <v>39.7849</v>
       </c>
-      <c r="O18" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P18" s="14" t="n">
+      <c r="O18" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P18" s="15" t="n">
         <v>0.2043</v>
       </c>
-      <c r="Q18" s="9" t="n">
+      <c r="Q18" s="10" t="n">
         <f aca="false">(L18/D18)*100</f>
         <v>100</v>
       </c>
-      <c r="R18" s="13" t="s">
+      <c r="R18" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S18" s="1"/>
-      <c r="T18" s="14" t="n">
+      <c r="T18" s="15" t="n">
         <v>94</v>
       </c>
-      <c r="U18" s="14" t="n">
+      <c r="U18" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V18" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W18" s="16" t="n">
+      <c r="V18" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W18" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X18" s="17" t="n">
+      <c r="X18" s="18" t="n">
         <v>41.4893</v>
       </c>
-      <c r="Y18" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z18" s="14" t="n">
+      <c r="Y18" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z18" s="15" t="n">
         <v>0.1702</v>
       </c>
-      <c r="AA18" s="9" t="n">
+      <c r="AA18" s="10" t="n">
         <f aca="false">(V18/D18)*100</f>
         <v>100</v>
       </c>
-      <c r="AB18" s="13" t="s">
+      <c r="AB18" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="n">
+      <c r="A19" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="9" t="n">
+      <c r="B19" s="10" t="n">
         <v>73</v>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D19" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E19" s="11" t="n">
+      <c r="D19" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E19" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F19" s="12" t="n">
+      <c r="F19" s="13" t="n">
         <v>41.0958</v>
       </c>
-      <c r="G19" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H19" s="9" t="n">
+      <c r="G19" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H19" s="10" t="n">
         <v>0.178</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="14" t="n">
+      <c r="J19" s="15" t="n">
         <v>78</v>
       </c>
-      <c r="K19" s="14" t="n">
+      <c r="K19" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="L19" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M19" s="16" t="n">
+      <c r="L19" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M19" s="17" t="n">
         <v>28</v>
       </c>
-      <c r="N19" s="17" t="n">
+      <c r="N19" s="18" t="n">
         <v>43.5897</v>
       </c>
-      <c r="O19" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P19" s="14" t="n">
+      <c r="O19" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P19" s="15" t="n">
         <v>0.1282</v>
       </c>
-      <c r="Q19" s="9" t="n">
+      <c r="Q19" s="10" t="n">
         <f aca="false">(L19/D19)*100</f>
         <v>100</v>
       </c>
-      <c r="R19" s="13" t="s">
+      <c r="R19" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S19" s="1"/>
-      <c r="T19" s="14" t="n">
+      <c r="T19" s="15" t="n">
         <v>89</v>
       </c>
-      <c r="U19" s="14" t="n">
+      <c r="U19" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="V19" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W19" s="16" t="n">
+      <c r="V19" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W19" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X19" s="17" t="n">
+      <c r="X19" s="18" t="n">
         <v>40.4494</v>
       </c>
-      <c r="Y19" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z19" s="14" t="n">
+      <c r="Y19" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z19" s="15" t="n">
         <v>0.191</v>
       </c>
-      <c r="AA19" s="9" t="n">
+      <c r="AA19" s="10" t="n">
         <f aca="false">(V19/D19)*100</f>
         <v>100</v>
       </c>
-      <c r="AB19" s="13" t="s">
+      <c r="AB19" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="n">
+      <c r="A20" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>77</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D20" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E20" s="11" t="n">
+      <c r="D20" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E20" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F20" s="12" t="n">
+      <c r="F20" s="13" t="n">
         <v>41.5584</v>
       </c>
-      <c r="G20" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H20" s="9" t="n">
+      <c r="G20" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H20" s="10" t="n">
         <v>0.1688</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="14" t="n">
+      <c r="J20" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="K20" s="14" t="n">
+      <c r="K20" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="L20" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M20" s="16" t="n">
+      <c r="L20" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M20" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N20" s="17" t="n">
+      <c r="N20" s="18" t="n">
         <v>42.9347</v>
       </c>
-      <c r="O20" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P20" s="14" t="n">
+      <c r="O20" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P20" s="15" t="n">
         <v>0.1413</v>
       </c>
-      <c r="Q20" s="9" t="n">
+      <c r="Q20" s="10" t="n">
         <f aca="false">(L20/D20)*100</f>
         <v>100</v>
       </c>
-      <c r="R20" s="13" t="s">
+      <c r="R20" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S20" s="1"/>
-      <c r="T20" s="14" t="n">
+      <c r="T20" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U20" s="14" t="n">
+      <c r="U20" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="V20" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W20" s="16" t="n">
+      <c r="V20" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W20" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X20" s="17" t="n">
+      <c r="X20" s="18" t="n">
         <v>40.7608</v>
       </c>
-      <c r="Y20" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z20" s="14" t="n">
+      <c r="Y20" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z20" s="15" t="n">
         <v>0.1847</v>
       </c>
-      <c r="AA20" s="9" t="n">
+      <c r="AA20" s="10" t="n">
         <f aca="false">(V20/D20)*100</f>
         <v>100</v>
       </c>
-      <c r="AB20" s="13" t="s">
+      <c r="AB20" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="n">
+      <c r="A21" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>71</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="D21" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" s="11" t="n">
+      <c r="D21" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F21" s="12" t="n">
+      <c r="F21" s="13" t="n">
         <v>44.3661</v>
       </c>
-      <c r="G21" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H21" s="9" t="n">
+      <c r="G21" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H21" s="10" t="n">
         <v>0.1126</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="14" t="n">
+      <c r="J21" s="15" t="n">
         <v>98</v>
       </c>
-      <c r="K21" s="14" t="n">
+      <c r="K21" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="L21" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M21" s="16" t="n">
+      <c r="L21" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M21" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N21" s="17" t="n">
+      <c r="N21" s="18" t="n">
         <v>40.3061</v>
       </c>
-      <c r="O21" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P21" s="14" t="n">
+      <c r="O21" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P21" s="15" t="n">
         <v>0.1938</v>
       </c>
-      <c r="Q21" s="9" t="n">
+      <c r="Q21" s="10" t="n">
         <f aca="false">(L21/D21)*100</f>
         <v>100</v>
       </c>
-      <c r="R21" s="13" t="s">
+      <c r="R21" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S21" s="1"/>
-      <c r="T21" s="14" t="n">
+      <c r="T21" s="15" t="n">
         <v>90</v>
       </c>
-      <c r="U21" s="14" t="n">
+      <c r="U21" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="V21" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W21" s="16" t="n">
+      <c r="V21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W21" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X21" s="17" t="n">
+      <c r="X21" s="18" t="n">
         <v>40.5555</v>
       </c>
-      <c r="Y21" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z21" s="14" t="n">
+      <c r="Y21" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z21" s="15" t="n">
         <v>0.1888</v>
       </c>
-      <c r="AA21" s="9" t="n">
+      <c r="AA21" s="10" t="n">
         <f aca="false">(V21/D21)*100</f>
         <v>100</v>
       </c>
-      <c r="AB21" s="13" t="s">
+      <c r="AB21" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="n">
+      <c r="A22" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="D22" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" s="11" t="n">
+      <c r="D22" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F22" s="12" t="n">
+      <c r="F22" s="13" t="n">
         <v>43.5714</v>
       </c>
-      <c r="G22" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H22" s="9" t="n">
+      <c r="G22" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H22" s="10" t="n">
         <v>0.1285</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="14" t="n">
+      <c r="J22" s="15" t="n">
         <v>88</v>
       </c>
-      <c r="K22" s="14" t="n">
+      <c r="K22" s="15" t="n">
         <v>14</v>
       </c>
-      <c r="L22" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M22" s="16" t="n">
+      <c r="L22" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M22" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N22" s="17" t="n">
+      <c r="N22" s="18" t="n">
         <v>42.0454</v>
       </c>
-      <c r="O22" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P22" s="14" t="n">
+      <c r="O22" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P22" s="15" t="n">
         <v>0.159</v>
       </c>
-      <c r="Q22" s="9" t="n">
+      <c r="Q22" s="10" t="n">
         <f aca="false">(L22/D22)*100</f>
         <v>100</v>
       </c>
-      <c r="R22" s="13" t="s">
+      <c r="R22" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S22" s="1"/>
-      <c r="T22" s="14" t="n">
+      <c r="T22" s="15" t="n">
         <v>88</v>
       </c>
-      <c r="U22" s="14" t="n">
+      <c r="U22" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V22" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W22" s="16" t="n">
+      <c r="V22" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W22" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X22" s="17" t="n">
+      <c r="X22" s="18" t="n">
         <v>40.909</v>
       </c>
-      <c r="Y22" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z22" s="14" t="n">
+      <c r="Y22" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z22" s="15" t="n">
         <v>0.1818</v>
       </c>
-      <c r="AA22" s="9" t="n">
+      <c r="AA22" s="10" t="n">
         <f aca="false">(V22/D22)*100</f>
         <v>100</v>
       </c>
-      <c r="AB22" s="13" t="s">
+      <c r="AB22" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="B23" s="9" t="n">
+      <c r="A23" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="B23" s="10" t="n">
         <v>75</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D23" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E23" s="11" t="n">
+      <c r="D23" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E23" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F23" s="12" t="n">
+      <c r="F23" s="13" t="n">
         <v>41.3333</v>
       </c>
-      <c r="G23" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H23" s="9" t="n">
+      <c r="G23" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H23" s="10" t="n">
         <v>0.1733</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="14" t="n">
+      <c r="J23" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="K23" s="14" t="n">
+      <c r="K23" s="15" t="n">
         <v>21</v>
       </c>
-      <c r="L23" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M23" s="16" t="n">
+      <c r="L23" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M23" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N23" s="17" t="n">
+      <c r="N23" s="18" t="n">
         <v>38.5869</v>
       </c>
-      <c r="O23" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P23" s="14" t="n">
+      <c r="O23" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P23" s="15" t="n">
         <v>0.2282</v>
       </c>
-      <c r="Q23" s="9" t="n">
+      <c r="Q23" s="10" t="n">
         <f aca="false">(L23/D23)*100</f>
         <v>100</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="R23" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S23" s="1"/>
-      <c r="T23" s="14" t="n">
+      <c r="T23" s="15" t="n">
         <v>90</v>
       </c>
-      <c r="U23" s="14" t="n">
+      <c r="U23" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V23" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W23" s="16" t="n">
+      <c r="V23" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W23" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X23" s="17" t="n">
+      <c r="X23" s="18" t="n">
         <v>41.1111</v>
       </c>
-      <c r="Y23" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z23" s="14" t="n">
+      <c r="Y23" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z23" s="15" t="n">
         <v>0.1777</v>
       </c>
-      <c r="AA23" s="9" t="n">
+      <c r="AA23" s="10" t="n">
         <f aca="false">(V23/D23)*100</f>
         <v>100</v>
       </c>
-      <c r="AB23" s="13" t="s">
+      <c r="AB23" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="n">
+      <c r="A24" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="10" t="n">
         <v>76</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="D24" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E24" s="11" t="n">
+      <c r="D24" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F24" s="12" t="n">
+      <c r="F24" s="13" t="n">
         <v>40.7894</v>
       </c>
-      <c r="G24" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H24" s="9" t="n">
+      <c r="G24" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H24" s="10" t="n">
         <v>0.1842</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="14" t="n">
+      <c r="J24" s="15" t="n">
         <v>91</v>
       </c>
-      <c r="K24" s="14" t="n">
+      <c r="K24" s="15" t="n">
         <v>14</v>
       </c>
-      <c r="L24" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M24" s="16" t="n">
+      <c r="L24" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M24" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N24" s="17" t="n">
+      <c r="N24" s="18" t="n">
         <v>42.3076</v>
       </c>
-      <c r="O24" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P24" s="14" t="n">
+      <c r="O24" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P24" s="15" t="n">
         <v>0.1538</v>
       </c>
-      <c r="Q24" s="9" t="n">
+      <c r="Q24" s="10" t="n">
         <f aca="false">(L24/D24)*100</f>
         <v>100</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="R24" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S24" s="1"/>
-      <c r="T24" s="14" t="n">
+      <c r="T24" s="15" t="n">
         <v>103</v>
       </c>
-      <c r="U24" s="14" t="n">
+      <c r="U24" s="15" t="n">
         <v>21</v>
       </c>
-      <c r="V24" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W24" s="16" t="n">
+      <c r="V24" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W24" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X24" s="17" t="n">
+      <c r="X24" s="18" t="n">
         <v>39.8058</v>
       </c>
-      <c r="Y24" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z24" s="14" t="n">
+      <c r="Y24" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z24" s="15" t="n">
         <v>0.2038</v>
       </c>
-      <c r="AA24" s="9" t="n">
+      <c r="AA24" s="10" t="n">
         <f aca="false">(V24/D24)*100</f>
         <v>100</v>
       </c>
-      <c r="AB24" s="13" t="s">
+      <c r="AB24" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="n">
+      <c r="A25" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="C25" s="9" t="n">
+      <c r="C25" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="D25" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E25" s="11" t="n">
+      <c r="D25" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E25" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F25" s="12" t="n">
+      <c r="F25" s="13" t="n">
         <v>37.8571</v>
       </c>
-      <c r="G25" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H25" s="9" t="n">
+      <c r="G25" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H25" s="10" t="n">
         <v>0.2428</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="14" t="n">
+      <c r="J25" s="15" t="n">
         <v>101</v>
       </c>
-      <c r="K25" s="14" t="n">
+      <c r="K25" s="15" t="n">
         <v>21</v>
       </c>
-      <c r="L25" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M25" s="16" t="n">
+      <c r="L25" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M25" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N25" s="17" t="n">
+      <c r="N25" s="18" t="n">
         <v>39.6039</v>
       </c>
-      <c r="O25" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P25" s="14" t="n">
+      <c r="O25" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P25" s="15" t="n">
         <v>0.2079</v>
       </c>
-      <c r="Q25" s="9" t="n">
+      <c r="Q25" s="10" t="n">
         <f aca="false">(L25/D25)*100</f>
         <v>100</v>
       </c>
-      <c r="R25" s="13" t="s">
+      <c r="R25" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S25" s="1"/>
-      <c r="T25" s="14" t="n">
+      <c r="T25" s="15" t="n">
         <v>105</v>
       </c>
-      <c r="U25" s="14" t="n">
+      <c r="U25" s="15" t="n">
         <v>25</v>
       </c>
-      <c r="V25" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W25" s="16" t="n">
+      <c r="V25" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W25" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X25" s="17" t="n">
+      <c r="X25" s="18" t="n">
         <v>38.0952</v>
       </c>
-      <c r="Y25" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z25" s="14" t="n">
+      <c r="Y25" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z25" s="15" t="n">
         <v>0.238</v>
       </c>
-      <c r="AA25" s="9" t="n">
+      <c r="AA25" s="10" t="n">
         <f aca="false">(V25/D25)*100</f>
         <v>100</v>
       </c>
-      <c r="AB25" s="13" t="s">
+      <c r="AB25" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="n">
+      <c r="A26" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="B26" s="9" t="n">
+      <c r="B26" s="10" t="n">
         <v>79</v>
       </c>
-      <c r="C26" s="9" t="n">
+      <c r="C26" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D26" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E26" s="11" t="n">
+      <c r="D26" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E26" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F26" s="12" t="n">
+      <c r="F26" s="13" t="n">
         <v>43.6708</v>
       </c>
-      <c r="G26" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H26" s="9" t="n">
+      <c r="G26" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H26" s="10" t="n">
         <v>0.1265</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="14" t="n">
+      <c r="J26" s="15" t="n">
         <v>90</v>
       </c>
-      <c r="K26" s="14" t="n">
+      <c r="K26" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="L26" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M26" s="16" t="n">
+      <c r="L26" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M26" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N26" s="17" t="n">
+      <c r="N26" s="18" t="n">
         <v>42.7777</v>
       </c>
-      <c r="O26" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P26" s="14" t="n">
+      <c r="O26" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P26" s="15" t="n">
         <v>0.1444</v>
       </c>
-      <c r="Q26" s="9" t="n">
+      <c r="Q26" s="10" t="n">
         <f aca="false">(L26/D26)*100</f>
         <v>100</v>
       </c>
-      <c r="R26" s="13" t="s">
+      <c r="R26" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S26" s="1"/>
-      <c r="T26" s="14" t="n">
+      <c r="T26" s="15" t="n">
         <v>105</v>
       </c>
-      <c r="U26" s="14" t="n">
+      <c r="U26" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="V26" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W26" s="16" t="n">
+      <c r="V26" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W26" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X26" s="17" t="n">
+      <c r="X26" s="18" t="n">
         <v>37.1428</v>
       </c>
-      <c r="Y26" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z26" s="14" t="n">
+      <c r="Y26" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z26" s="15" t="n">
         <v>0.2571</v>
       </c>
-      <c r="AA26" s="9" t="n">
+      <c r="AA26" s="10" t="n">
         <f aca="false">(V26/D26)*100</f>
         <v>100</v>
       </c>
-      <c r="AB26" s="13" t="s">
+      <c r="AB26" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="n">
+      <c r="A27" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="B27" s="9" t="n">
+      <c r="B27" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D27" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E27" s="11" t="n">
+      <c r="D27" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E27" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F27" s="12" t="n">
+      <c r="F27" s="13" t="n">
         <v>40.7142</v>
       </c>
-      <c r="G27" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H27" s="9" t="n">
+      <c r="G27" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H27" s="10" t="n">
         <v>0.1857</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="J27" s="14" t="n">
+      <c r="J27" s="15" t="n">
         <v>97</v>
       </c>
-      <c r="K27" s="14" t="n">
+      <c r="K27" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="L27" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M27" s="16" t="n">
+      <c r="L27" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M27" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N27" s="17" t="n">
+      <c r="N27" s="18" t="n">
         <v>41.7525</v>
       </c>
-      <c r="O27" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P27" s="14" t="n">
+      <c r="O27" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P27" s="15" t="n">
         <v>0.1649</v>
       </c>
-      <c r="Q27" s="9" t="n">
+      <c r="Q27" s="10" t="n">
         <f aca="false">(L27/D27)*100</f>
         <v>100</v>
       </c>
-      <c r="R27" s="13" t="s">
+      <c r="R27" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S27" s="1"/>
-      <c r="T27" s="14" t="n">
+      <c r="T27" s="15" t="n">
         <v>87</v>
       </c>
-      <c r="U27" s="14" t="n">
+      <c r="U27" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="V27" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W27" s="16" t="n">
+      <c r="V27" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W27" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X27" s="17" t="n">
+      <c r="X27" s="18" t="n">
         <v>43.1034</v>
       </c>
-      <c r="Y27" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z27" s="14" t="n">
+      <c r="Y27" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z27" s="15" t="n">
         <v>0.1379</v>
       </c>
-      <c r="AA27" s="9" t="n">
+      <c r="AA27" s="10" t="n">
         <f aca="false">(V27/D27)*100</f>
         <v>100</v>
       </c>
-      <c r="AB27" s="13" t="s">
+      <c r="AB27" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="n">
+      <c r="A28" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="B28" s="9" t="n">
+      <c r="B28" s="10" t="n">
         <v>77</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D28" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E28" s="11" t="n">
+      <c r="D28" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E28" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F28" s="12" t="n">
+      <c r="F28" s="13" t="n">
         <v>41.5584</v>
       </c>
-      <c r="G28" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H28" s="9" t="n">
+      <c r="G28" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H28" s="10" t="n">
         <v>0.1688</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="14" t="n">
+      <c r="J28" s="15" t="n">
         <v>85</v>
       </c>
-      <c r="K28" s="14" t="n">
+      <c r="K28" s="15" t="n">
         <v>11</v>
       </c>
-      <c r="L28" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M28" s="16" t="n">
+      <c r="L28" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M28" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N28" s="17" t="n">
+      <c r="N28" s="18" t="n">
         <v>43.5294</v>
       </c>
-      <c r="O28" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P28" s="14" t="n">
+      <c r="O28" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P28" s="15" t="n">
         <v>0.1294</v>
       </c>
-      <c r="Q28" s="9" t="n">
+      <c r="Q28" s="10" t="n">
         <f aca="false">(L28/D28)*100</f>
         <v>100</v>
       </c>
-      <c r="R28" s="13" t="s">
+      <c r="R28" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S28" s="1"/>
-      <c r="T28" s="14" t="n">
+      <c r="T28" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U28" s="14" t="n">
+      <c r="U28" s="15" t="n">
         <v>21</v>
       </c>
-      <c r="V28" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W28" s="16" t="n">
+      <c r="V28" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W28" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X28" s="17" t="n">
+      <c r="X28" s="18" t="n">
         <v>38.5869</v>
       </c>
-      <c r="Y28" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z28" s="14" t="n">
+      <c r="Y28" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z28" s="15" t="n">
         <v>0.2282</v>
       </c>
-      <c r="AA28" s="9" t="n">
+      <c r="AA28" s="10" t="n">
         <f aca="false">(V28/D28)*100</f>
         <v>100</v>
       </c>
-      <c r="AB28" s="13" t="s">
+      <c r="AB28" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="n">
+      <c r="A29" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="B29" s="9" t="n">
+      <c r="B29" s="10" t="n">
         <v>78</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="D29" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E29" s="11" t="n">
+      <c r="D29" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E29" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F29" s="12" t="n">
+      <c r="F29" s="13" t="n">
         <v>39.1025</v>
       </c>
-      <c r="G29" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H29" s="9" t="n">
+      <c r="G29" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H29" s="10" t="n">
         <v>0.2179</v>
       </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="14" t="n">
+      <c r="J29" s="15" t="n">
         <v>89</v>
       </c>
-      <c r="K29" s="14" t="n">
+      <c r="K29" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="L29" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M29" s="16" t="n">
+      <c r="L29" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M29" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N29" s="17" t="n">
+      <c r="N29" s="18" t="n">
         <v>40.4494</v>
       </c>
-      <c r="O29" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P29" s="14" t="n">
+      <c r="O29" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P29" s="15" t="n">
         <v>0.191</v>
       </c>
-      <c r="Q29" s="9" t="n">
+      <c r="Q29" s="10" t="n">
         <f aca="false">(L29/D29)*100</f>
         <v>100</v>
       </c>
-      <c r="R29" s="13" t="s">
+      <c r="R29" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S29" s="1"/>
-      <c r="T29" s="14" t="n">
+      <c r="T29" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U29" s="14" t="n">
+      <c r="U29" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="V29" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W29" s="16" t="n">
+      <c r="V29" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W29" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X29" s="17" t="n">
+      <c r="X29" s="18" t="n">
         <v>40.2173</v>
       </c>
-      <c r="Y29" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z29" s="14" t="n">
+      <c r="Y29" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z29" s="15" t="n">
         <v>0.1956</v>
       </c>
-      <c r="AA29" s="9" t="n">
+      <c r="AA29" s="10" t="n">
         <f aca="false">(V29/D29)*100</f>
         <v>100</v>
       </c>
-      <c r="AB29" s="13" t="s">
+      <c r="AB29" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="10" t="n">
         <v>27</v>
       </c>
-      <c r="B30" s="9" t="n">
+      <c r="B30" s="10" t="n">
         <v>81</v>
       </c>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D30" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E30" s="11" t="n">
+      <c r="D30" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E30" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F30" s="12" t="n">
+      <c r="F30" s="13" t="n">
         <v>41.9753</v>
       </c>
-      <c r="G30" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H30" s="9" t="n">
+      <c r="G30" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H30" s="10" t="n">
         <v>0.1604</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="14" t="n">
+      <c r="J30" s="15" t="n">
         <v>96</v>
       </c>
-      <c r="K30" s="14" t="n">
+      <c r="K30" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="L30" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M30" s="16" t="n">
+      <c r="L30" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M30" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N30" s="17" t="n">
+      <c r="N30" s="18" t="n">
         <v>40.1041</v>
       </c>
-      <c r="O30" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P30" s="14" t="n">
+      <c r="O30" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P30" s="15" t="n">
         <v>0.1979</v>
       </c>
-      <c r="Q30" s="9" t="n">
+      <c r="Q30" s="10" t="n">
         <f aca="false">(L30/D30)*100</f>
         <v>100</v>
       </c>
-      <c r="R30" s="13" t="s">
+      <c r="R30" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S30" s="1"/>
-      <c r="T30" s="14" t="n">
+      <c r="T30" s="15" t="n">
         <v>87</v>
       </c>
-      <c r="U30" s="14" t="n">
+      <c r="U30" s="15" t="n">
         <v>11</v>
       </c>
-      <c r="V30" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W30" s="16" t="n">
+      <c r="V30" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W30" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="X30" s="17" t="n">
+      <c r="X30" s="18" t="n">
         <v>43.6781</v>
       </c>
-      <c r="Y30" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z30" s="14" t="n">
+      <c r="Y30" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z30" s="15" t="n">
         <v>0.1264</v>
       </c>
-      <c r="AA30" s="9" t="n">
+      <c r="AA30" s="10" t="n">
         <f aca="false">(V30/D30)*100</f>
         <v>100</v>
       </c>
-      <c r="AB30" s="13" t="s">
+      <c r="AB30" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
+      <c r="A31" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="B31" s="9" t="n">
+      <c r="B31" s="10" t="n">
         <v>73</v>
       </c>
-      <c r="C31" s="9" t="n">
+      <c r="C31" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="D31" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E31" s="11" t="n">
+      <c r="D31" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E31" s="12" t="n">
         <v>12.5</v>
       </c>
-      <c r="F31" s="12" t="n">
+      <c r="F31" s="13" t="n">
         <v>42.4657</v>
       </c>
-      <c r="G31" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H31" s="9" t="n">
+      <c r="G31" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H31" s="10" t="n">
         <v>0.1506</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="14" t="n">
+      <c r="J31" s="15" t="n">
         <v>91</v>
       </c>
-      <c r="K31" s="14" t="n">
+      <c r="K31" s="15" t="n">
         <v>15</v>
       </c>
-      <c r="L31" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M31" s="16" t="n">
+      <c r="L31" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M31" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N31" s="17" t="n">
+      <c r="N31" s="18" t="n">
         <v>41.7582</v>
       </c>
-      <c r="O31" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P31" s="14" t="n">
+      <c r="O31" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P31" s="15" t="n">
         <v>0.1648</v>
       </c>
-      <c r="Q31" s="9" t="n">
+      <c r="Q31" s="10" t="n">
         <f aca="false">(L31/D31)*100</f>
         <v>100</v>
       </c>
-      <c r="R31" s="13" t="s">
+      <c r="R31" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S31" s="1"/>
-      <c r="T31" s="14" t="n">
+      <c r="T31" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U31" s="14" t="n">
-        <v>20</v>
-      </c>
-      <c r="V31" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W31" s="16" t="n">
+      <c r="U31" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="V31" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W31" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X31" s="17" t="n">
+      <c r="X31" s="18" t="n">
         <v>39.1304</v>
       </c>
-      <c r="Y31" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z31" s="14" t="n">
+      <c r="Y31" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z31" s="15" t="n">
         <v>0.2173</v>
       </c>
-      <c r="AA31" s="9" t="n">
+      <c r="AA31" s="10" t="n">
         <f aca="false">(V31/D31)*100</f>
         <v>100</v>
       </c>
-      <c r="AB31" s="13" t="s">
+      <c r="AB31" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="n">
+      <c r="A32" s="10" t="n">
         <v>29</v>
       </c>
-      <c r="B32" s="9" t="n">
+      <c r="B32" s="10" t="n">
         <v>72</v>
       </c>
-      <c r="C32" s="9" t="n">
+      <c r="C32" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D32" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E32" s="11" t="n">
+      <c r="D32" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E32" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F32" s="12" t="n">
+      <c r="F32" s="13" t="n">
         <v>40.9722</v>
       </c>
-      <c r="G32" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H32" s="9" t="n">
+      <c r="G32" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H32" s="10" t="n">
         <v>0.1805</v>
       </c>
       <c r="I32" s="1"/>
-      <c r="J32" s="14" t="n">
+      <c r="J32" s="15" t="n">
         <v>104</v>
       </c>
-      <c r="K32" s="14" t="n">
+      <c r="K32" s="15" t="n">
         <v>28</v>
       </c>
-      <c r="L32" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M32" s="16" t="n">
+      <c r="L32" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M32" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="N32" s="17" t="n">
+      <c r="N32" s="18" t="n">
         <v>36.5384</v>
       </c>
-      <c r="O32" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P32" s="14" t="n">
+      <c r="O32" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P32" s="15" t="n">
         <v>0.2692</v>
       </c>
-      <c r="Q32" s="9" t="n">
+      <c r="Q32" s="10" t="n">
         <f aca="false">(L32/D32)*100</f>
         <v>100</v>
       </c>
-      <c r="R32" s="13" t="s">
+      <c r="R32" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S32" s="1"/>
-      <c r="T32" s="14" t="n">
+      <c r="T32" s="15" t="n">
         <v>92</v>
       </c>
-      <c r="U32" s="14" t="n">
+      <c r="U32" s="15" t="n">
         <v>15</v>
       </c>
-      <c r="V32" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W32" s="16" t="n">
+      <c r="V32" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W32" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="X32" s="17" t="n">
+      <c r="X32" s="18" t="n">
         <v>41.8478</v>
       </c>
-      <c r="Y32" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z32" s="14" t="n">
+      <c r="Y32" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z32" s="15" t="n">
         <v>0.163</v>
       </c>
-      <c r="AA32" s="9" t="n">
+      <c r="AA32" s="10" t="n">
         <f aca="false">(V32/D32)*100</f>
         <v>100</v>
       </c>
-      <c r="AB32" s="13" t="s">
+      <c r="AB32" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="n">
+      <c r="A33" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="B33" s="9" t="n">
+      <c r="B33" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="C33" s="9" t="n">
+      <c r="C33" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="D33" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E33" s="11" t="n">
+      <c r="D33" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E33" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="F33" s="12" t="n">
+      <c r="F33" s="13" t="n">
         <v>38.125</v>
       </c>
-      <c r="G33" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H33" s="9" t="n">
+      <c r="G33" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H33" s="10" t="n">
         <v>0.2375</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="14" t="n">
+      <c r="J33" s="15" t="n">
         <v>97</v>
       </c>
-      <c r="K33" s="14" t="n">
+      <c r="K33" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="L33" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M33" s="16" t="n">
+      <c r="L33" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M33" s="17" t="n">
         <v>12.5</v>
       </c>
-      <c r="N33" s="17" t="n">
+      <c r="N33" s="18" t="n">
         <v>38.6597</v>
       </c>
-      <c r="O33" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="P33" s="14" t="n">
+      <c r="O33" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="P33" s="15" t="n">
         <v>0.2268</v>
       </c>
-      <c r="Q33" s="9" t="n">
+      <c r="Q33" s="10" t="n">
         <f aca="false">(L33/D33)*100</f>
         <v>100</v>
       </c>
-      <c r="R33" s="13" t="s">
+      <c r="R33" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S33" s="1"/>
-      <c r="T33" s="14" t="n">
+      <c r="T33" s="15" t="n">
         <v>83</v>
       </c>
-      <c r="U33" s="14" t="n">
+      <c r="U33" s="15" t="n">
         <v>11</v>
       </c>
-      <c r="V33" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="W33" s="16" t="n">
+      <c r="V33" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="W33" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="X33" s="17" t="n">
+      <c r="X33" s="18" t="n">
         <v>43.3734</v>
       </c>
-      <c r="Y33" s="16" t="n">
-        <v>50</v>
-      </c>
-      <c r="Z33" s="14" t="n">
+      <c r="Y33" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z33" s="15" t="n">
         <v>0.1325</v>
       </c>
-      <c r="AA33" s="9" t="n">
+      <c r="AA33" s="10" t="n">
         <f aca="false">(V33/D33)*100</f>
         <v>100</v>
       </c>
-      <c r="AB33" s="13" t="s">
+      <c r="AB33" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2996,27 +3029,27 @@
         <f aca="false">SUM(C4:C33)</f>
         <v>391</v>
       </c>
-      <c r="D34" s="19" t="n">
+      <c r="D34" s="20" t="n">
         <f aca="false">SUM(D4:D33)</f>
         <v>600</v>
       </c>
-      <c r="E34" s="20" t="n">
+      <c r="E34" s="21" t="n">
         <f aca="false">SUM(E4:E33)</f>
         <v>562.5</v>
       </c>
-      <c r="F34" s="21" t="n">
+      <c r="F34" s="22" t="n">
         <f aca="false">SUM(F4:F33)</f>
         <v>1237.2269</v>
       </c>
-      <c r="G34" s="22" t="n">
+      <c r="G34" s="23" t="n">
         <f aca="false">SUM(G4:G33)</f>
         <v>1500</v>
       </c>
-      <c r="H34" s="23" t="n">
+      <c r="H34" s="24" t="n">
         <f aca="false">SUM(H4:H33)</f>
         <v>5.2609</v>
       </c>
-      <c r="I34" s="24"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="4" t="n">
         <f aca="false">SUM(J4:J33)</f>
         <v>2791</v>
@@ -3025,23 +3058,23 @@
         <f aca="false">SUM(K4:K33)</f>
         <v>526</v>
       </c>
-      <c r="L34" s="19" t="n">
+      <c r="L34" s="20" t="n">
         <f aca="false">SUM(L4:L33)</f>
         <v>600</v>
       </c>
-      <c r="M34" s="21" t="n">
+      <c r="M34" s="22" t="n">
         <f aca="false">SUM(M4:M33)</f>
         <v>592</v>
       </c>
-      <c r="N34" s="21" t="n">
+      <c r="N34" s="22" t="n">
         <f aca="false">SUM(N4:N33)</f>
         <v>1219.6896</v>
       </c>
-      <c r="O34" s="21" t="n">
+      <c r="O34" s="22" t="n">
         <f aca="false">SUM(O4:O33)</f>
         <v>1500</v>
       </c>
-      <c r="P34" s="23" t="n">
+      <c r="P34" s="24" t="n">
         <f aca="false">SUM(P4:P33)</f>
         <v>5.605</v>
       </c>
@@ -3050,7 +3083,7 @@
         <v>3000</v>
       </c>
       <c r="R34" s="4"/>
-      <c r="S34" s="5"/>
+      <c r="S34" s="6"/>
       <c r="T34" s="4" t="n">
         <f aca="false">SUM(T4:T33)</f>
         <v>2748</v>
@@ -3059,23 +3092,23 @@
         <f aca="false">SUM(U4:U33)</f>
         <v>506</v>
       </c>
-      <c r="V34" s="19" t="n">
+      <c r="V34" s="20" t="n">
         <f aca="false">SUM(V4:V33)</f>
         <v>600</v>
       </c>
-      <c r="W34" s="21" t="n">
+      <c r="W34" s="22" t="n">
         <f aca="false">SUM(W4:W33)</f>
         <v>615.5</v>
       </c>
-      <c r="X34" s="21" t="n">
+      <c r="X34" s="22" t="n">
         <f aca="false">SUM(X4:X33)</f>
         <v>1225.5153</v>
       </c>
-      <c r="Y34" s="21" t="n">
+      <c r="Y34" s="22" t="n">
         <f aca="false">SUM(Y4:Y33)</f>
         <v>1500</v>
       </c>
-      <c r="Z34" s="23" t="n">
+      <c r="Z34" s="24" t="n">
         <f aca="false">SUM(Z4:Z33)</f>
         <v>5.4881</v>
       </c>
@@ -3083,108 +3116,108 @@
         <f aca="false">SUM(AA4:AA33)</f>
         <v>3000</v>
       </c>
-      <c r="AB34" s="8"/>
+      <c r="AB34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="20" t="n">
+      <c r="B35" s="21" t="n">
         <f aca="false">B34/30</f>
         <v>74.3666666666667</v>
       </c>
-      <c r="C35" s="19" t="n">
+      <c r="C35" s="20" t="n">
         <f aca="false">C34/30</f>
         <v>13.0333333333333</v>
       </c>
-      <c r="D35" s="19" t="n">
+      <c r="D35" s="20" t="n">
         <f aca="false">D34/30</f>
         <v>20</v>
       </c>
-      <c r="E35" s="25" t="n">
+      <c r="E35" s="26" t="n">
         <f aca="false">E34/30</f>
         <v>18.75</v>
       </c>
-      <c r="F35" s="21" t="n">
+      <c r="F35" s="22" t="n">
         <f aca="false">F34/30</f>
         <v>41.2408966666667</v>
       </c>
-      <c r="G35" s="26" t="n">
+      <c r="G35" s="27" t="n">
         <f aca="false">G34/30</f>
         <v>50</v>
       </c>
-      <c r="H35" s="23" t="n">
+      <c r="H35" s="24" t="n">
         <f aca="false">H34/30</f>
         <v>0.175363333333333</v>
       </c>
-      <c r="I35" s="24"/>
-      <c r="J35" s="20" t="n">
+      <c r="I35" s="25"/>
+      <c r="J35" s="21" t="n">
         <f aca="false">J34/30</f>
         <v>93.0333333333333</v>
       </c>
-      <c r="K35" s="19" t="n">
+      <c r="K35" s="20" t="n">
         <f aca="false">K34/30</f>
         <v>17.5333333333333</v>
       </c>
-      <c r="L35" s="19" t="n">
+      <c r="L35" s="20" t="n">
         <f aca="false">L34/30</f>
         <v>20</v>
       </c>
-      <c r="M35" s="21" t="n">
+      <c r="M35" s="22" t="n">
         <f aca="false">M34/30</f>
         <v>19.7333333333333</v>
       </c>
-      <c r="N35" s="21" t="n">
+      <c r="N35" s="22" t="n">
         <f aca="false">N34/30</f>
         <v>40.65632</v>
       </c>
-      <c r="O35" s="19" t="n">
+      <c r="O35" s="20" t="n">
         <f aca="false">O34/30</f>
         <v>50</v>
       </c>
-      <c r="P35" s="23" t="n">
+      <c r="P35" s="24" t="n">
         <f aca="false">P34/30</f>
         <v>0.186833333333333</v>
       </c>
-      <c r="Q35" s="20" t="n">
+      <c r="Q35" s="21" t="n">
         <f aca="false">Q34/30</f>
         <v>100</v>
       </c>
-      <c r="R35" s="27"/>
-      <c r="S35" s="28"/>
-      <c r="T35" s="20" t="n">
+      <c r="R35" s="28"/>
+      <c r="S35" s="29"/>
+      <c r="T35" s="21" t="n">
         <f aca="false">T34/30</f>
         <v>91.6</v>
       </c>
-      <c r="U35" s="19" t="n">
+      <c r="U35" s="20" t="n">
         <f aca="false">U34/30</f>
         <v>16.8666666666667</v>
       </c>
-      <c r="V35" s="19" t="n">
+      <c r="V35" s="20" t="n">
         <f aca="false">V34/30</f>
         <v>20</v>
       </c>
-      <c r="W35" s="21" t="n">
+      <c r="W35" s="22" t="n">
         <f aca="false">W34/30</f>
         <v>20.5166666666667</v>
       </c>
-      <c r="X35" s="21" t="n">
+      <c r="X35" s="22" t="n">
         <f aca="false">X34/30</f>
         <v>40.85051</v>
       </c>
-      <c r="Y35" s="19" t="n">
+      <c r="Y35" s="20" t="n">
         <f aca="false">Y34/30</f>
         <v>50</v>
       </c>
-      <c r="Z35" s="23" t="n">
+      <c r="Z35" s="24" t="n">
         <f aca="false">Z34/30</f>
         <v>0.182936666666667</v>
       </c>
-      <c r="AA35" s="20" t="n">
+      <c r="AA35" s="21" t="n">
         <f aca="false">AA34/30</f>
         <v>100</v>
       </c>
-      <c r="AB35" s="27"/>
+      <c r="AB35" s="28"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
@@ -3197,7 +3230,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
-      <c r="D39" s="29"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>

</xml_diff>